<commit_message>
Get daily reddit data: Tue Jul 15 08:13:58 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_20.xlsx
+++ b/data/collected_data/2025_07_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C506"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3491 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1m0bq6f</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Summer 💅</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s4hoyaaptzcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1m0a73u</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>New Set - Funky French Tips</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h87y8hjczcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1m09647</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>This One’s Getting Out of Hand—Some Love It, Some Hate It. WYT? 🔩💅</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m09647</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1m08uxi</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Would you call my nail beds more flat or sculpted as far as Gel-X nail tips go?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m08uxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1m07zqo</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Should I ask to redo? Inspo pic: @maiellajackson on ig</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m07zqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1m06ld9</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>first time using acrylic!!</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m06ld9</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1m07vgp</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Are my nails too short to do almond shape?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ohycwuyoycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1m077rx</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>My nails have never looked or grown better!</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ea22v8vxiycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1m06vfc</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Best nail shape for my hand?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs0pic1ufycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1m06rw9</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>I’ve found my wedding nails!!</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8epdkgcyeycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1m06qs8</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Really happy with this set</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s0uzj4oeycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1m06lsh</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Watermelon 🍉 Photoshoot</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m06lsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1m06ezv</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Too thick for a BIAB?</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m06ezv</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1m051ya</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Nail kit for my girlfriend?</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m051ya/nail_kit_for_my_girlfriend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1m05khh</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Inspired by the Sopranos TV show 🖤⭐️🦆🩸</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m05khh</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1m05lea</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>What hand shape am I? And therefore what nail shape should I get?</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m05lea</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1m057gz</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>I hate the nail color I got :( it’s too…Easter….</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m057gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1m050kx</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>I’m afraid to ask</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m050kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1m04w4z</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>My nail artist wanted to do this set for a discount, I love them</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m04w4z</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1m04qzd</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Gloomy Bear claws!</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m04qzd</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1m04cq5</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>I did these 🥰😍</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx69b3xhuxcf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1m04c3v</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Animal Print Black</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rkmecqtauxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1m048ko</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>what should I name these??</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dl4q7vnjtxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1m046eg</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>what should the base color be?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xuok9ho1txcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1m042nw</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>press ons</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x40ssc8sxcf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1m03z2f</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>best nail glue for press ons?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m03z2f/best_nail_glue_for_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1m03or5</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>I got myself some new nail polish! Learning to manicure at home</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fjn9rvp1pxcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1m03b6f</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>DIY gel mani done yesterday, followed instructions to a T, and I can still make an indent/scratch on my nails!? Help me understand where I’m going wrong!</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/081u3rsxlxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1m02xx4</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>First manicure in over a year!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m02xx4</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1m02wp0</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>it’s rare when the thumb is my favourite nail of the set🌷✨</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m02wp0</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1m02jwq</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>My girl killed the sushi nails today !</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m02jwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1m02hf1</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>I did these nails today! I was fascinated with the result 🥹</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/shnr2v8cfxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1m025ti</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>What am i doing wrong??</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9urpmf0ucxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1m01xjx</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Thin nails/damage</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzbyscg3bxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1m025v0</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>My best work yet</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kywlqfhucxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1m01m28</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Non-Gel Options</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m01m28/nongel_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1m01nfb</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Wet n wild - nuclear war</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m01nfb</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1m01ggp</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Opinions Wanted 😊</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjmt9gvi7xcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1m01bu0</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>How can I get my hands on Wilde Pedique products without being a pro in the UK?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m01bu0/how_can_i_get_my_hands_on_wilde_pedique_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1m015gm</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>how much would you charge/expect to be charged for this set?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m015gm</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1m00xcr</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Practice set</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m00xcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1lzxblk</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Tips - Moisture Under Press Ons</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzxblk/tips_moisture_under_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1m006fm</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Super happy with the result!</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m006fm</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1lzzseu</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>my most perfect manicure !</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gkxnjvkevwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1lzzlhu</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Anyone know what's a great uv/LED drying top coat for acrylics ?</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzzlhu/anyone_know_whats_a_great_uvled_drying_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1lzzlfz</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Busted 3 nails this weekend! Longest my natural nails have ever been but it's time to let go 😔</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzzlfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1lzygvj</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Nothing stays on</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzygvj/nothing_stays_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1lzz5ql</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Thought I’d try orange 🧡</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/04s4rkd5rwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1lzyy8b</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Has this happen to anyone?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ai7wtzopwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1lzyd3b</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Summer Fish 🐟</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzyd3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1lzycwj</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Nails too long?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzycwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1lzyaru</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Butter Yellow ✨</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzyaru</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1lzy9ek</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Help! I got regular nail polish on my gel nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mdql5wlkwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1lzxubm</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>Dip powder</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzxubm/dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1lzxd55</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nail Salon Swatches</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzxd55/nail_salon_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1lzx88o</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>3rd time using builder gelli</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzx88o</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1lzx2cl</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Fresh Set Alert! Tried a New Style for My Mani—What Do You Think?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzx2cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1lzvmst</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Stray Kids inspired nails!⛓️🩸</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzvmst</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1lzvp51</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Pink Pony Club nails 🦄</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/900cf58r3wcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1lzvh3k</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Rant</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzvh3k/rant/</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1lzvghj</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Finally splurged on a fancymani</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t15rbcm62wcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1lzvek0</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>My second attempt at butterfly nails 3 years later! What do you think?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzvek0</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1lzvbof</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>New nails are gorgeous</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzvbof</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1lztzzk</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>First time extensions.. Are they okay?</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lztzzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1lzv17x</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>New design</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0h1e5w8hzvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1lzv08y</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Press on nails brand from Europe ?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzv08y</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1lztym1</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Cat eye on nails ✨</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lztym1</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1lzsrjb</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Gigi inspired</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ysrx6bqkvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1lzsu9e</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Canada Days nails.</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llbnv908lvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1lzsdda</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Need some tips</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0j14bqi5ivcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1lzs9g7</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>What's the best way to temporarily fix this break? My nail appointment got moved to next week so I have to deal with this for a few more days.</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8oy0lcghvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1lzp2td</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>New to Gel Nails- Question about Nail Growth</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzp2td</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1lzpxjw</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Miss wearing sandals</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzpxjw/miss_wearing_sandals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1lzpows</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Finally did my nails after a year of doing nothing</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opmfjyxh0vcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1lzq7rh</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Disconfort days after manicure</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzq7rh/disconfort_days_after_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1lzqs1p</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Love this fairy gel mani!</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzqs1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1lzrrsg</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Sparkly shorties</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t9qeq1ydvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1lzr7ok</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Did you like my nails? It's the first time I've done them gold 😻🙌. They shine brighter than the sun!! 🌞</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzr7ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1lzr6rp</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Does this shape/length suit me?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzr6rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1lzqyol</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Can I use Deco Beauty nail stickers with Luminary and DND gel polishes?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fazq6tkw8vcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1lzpsfl</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Ready to do my nails on my own</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzpsfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1lzp7rm</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>New to Gel Nails- Question about Nail Growth</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzp7rm</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1lzp6s6</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Decided to try a new idea</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lxzv845xucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1lzp4ss</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>enough flowers for every day of the week</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eygoav1jwucf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1lzp2c9</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>I created a color coded system for my flower petal brushes - do you have any organizational hacks to share? New to nails and love it, but hate digging for stuff</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzp2c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1lzoz8d</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>They turned out super cute, what do you think?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znyna7rpvucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1lzovj1</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Just a sad rant</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzovj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1lzouuw</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Just a sad rant</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzouuw</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1lzoto2</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>First time using dual forms</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02ojp8dnuucf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1lzotrq</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Summer Set</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7ck6x6ouucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1lzot5r</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Please tell me if these are too long/not attractive</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/llprn7tjuucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1lznot2</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>my superman nails for the new movie!</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lznot2</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1lzmzgl</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o5acji1phucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1lzojtq</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Practicing my skills. Hoping to become a nail tech by age 19. 😅</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzojtq</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1lzojpt</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I wanted care bear nails</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0bzwgsrsucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1lzoeyo</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Was I Ok with my tip?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzoeyo/was_i_ok_with_my_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1lzo6a9</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>My new beach set 🐚🦀🌊 I am so obsessed and can’t stop staring at my hands!</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzo6a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1lzo5q5</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Has this always been a thing?</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1lzo5q5/has_this_always_been_a_thing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1lznvkv</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>First time getting acrylics!! Opinions??</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lznvkv</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1lznncu</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>WIP 🫶</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enejgpujmucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1m0azxp</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>"Jumpy" magnetic polish 😯🤨</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0azxp/jumpy_magnetic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1m09xgv</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Am I applying wrong?</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m09xgv/am_i_applying_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1m09fmm</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>US bound - indie purchases?</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m09fmm/us_bound_indie_purchases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1m096d2</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Peeling Nails &amp; Base Coat..</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m096d2/peeling_nails_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1m094fi</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Three day old magnetic mani (mixed techniques)</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/onadjat41zcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1m08wq5</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Best stamping nail polishes?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m08wq5/best_stamping_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1m08rn4</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Inspired by u/blackberryraccoon- celestial nails!</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m08rn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1m08np0</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Risks of developing allergies to regular polish?</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m08np0/risks_of_developing_allergies_to_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1m083l9</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Polish – Cherries &amp; Berries (PBE 2025 Exclusive)</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m083l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1m06zlx</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Did anyone else order as soon as it was available?</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j837s3avgycf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1m06wsg</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>70s vibes!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ud0r7sq5gycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1m06oww</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Polish – Butterball (PBE 2025 Exclusive)</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m06oww</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1m06nka</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>guess the polish</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m06nka</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1m06721</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Does anyone know a good dupe for I Scream Party?</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vxksbju9ycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1m05fol</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Some cool nail designs I did</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69nhalmg3ycf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1m04yql</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Aspen</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m04yql</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1m04s4x</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>sinful colors pride glitter dupe?</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m04s4x/sinful_colors_pride_glitter_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1m04r4h</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Just a couple of PPU rewind scores</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzc1yu1sxxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1m04il8</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Battle of the Boxes -Cuticula</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m04il8</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1m04e15</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>✨️🌈Glitter Zigs &amp; Zags🌈✨️</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m04e15</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1m0499y</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>It's just so pretty 😍</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0499y</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1m041wk</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Of fronds and vines and leaves and sedge and SNAILS</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m041wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1m03tzp</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Tips for getting a glassy finish on flaky polish</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l4wn3qg8qxcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1m03585</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Oceanic Forces 🌊</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y2pc8ulkxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1m02xyf</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Cadillacquer- Little Things</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m02xyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1m02ha7</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>She’s shifty 👀</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mg54jl7pexcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1m028pz</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>I can't believe these were $1.25 each</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m028pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1m01bpq</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Happy strawberry season! 🍓🍓🍓</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m01bpq</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1m00ujx</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Ok LA Colors, you did right by me this time</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m00ujx</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1m00kui</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Cadillacquer Neon Lights</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbsm2gc41xcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1m00gtv</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Help finding dupe?</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m00gtv/help_finding_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1m0012q</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>OPI - flex on the beach</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0012q</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1lzzvtg</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Keeping it simple for once</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38cwu7m7wwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1lzyzhk</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Anyone tried this?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sds2nfjxpwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1lzytw0</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Lacrimosa BKL</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdho127vowcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1lzylt1</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Gardening and Farming Lacqueristas - what's your routine like?</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzylt1/gardening_and_farming_lacqueristas_whats_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1lzy0wf</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Chopstix and Stones but green?</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzy0wf/chopstix_and_stones_but_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1lzxypg</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Help finding a neon pink</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzxypg/help_finding_a_neon_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1lzxsjw</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Results of the Lego spinny machine</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z7fng15phwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1lzxott</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Weird effect with thermals</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8lrxah0hwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1lzxn7b</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>iso a new red</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzxn7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1lzxcyl</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>What do y’all do when you go on vacation re: maintaining your manicure?</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzxcyl/what_do_yall_do_when_you_go_on_vacation_re/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1lzxcwl</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Trying out a new technique</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/UeNmufc.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1lzwrba</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Which magnet should I get?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjxchwftawcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1lzvqwn</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Top color altering polish?</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cp61kur24wcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1lzvjqj</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Crystal Knockout Torch of Affluence</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzvjqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1lzvgwl</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Over the moon</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzvgwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1lzv7se</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>My second attempt at butterfly nails 3 years later! What do you think?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzv7se</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1lzv1xg</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Make chrome powder stick and get chome-y?</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzv1xg/make_chrome_powder_stick_and_get_chomey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1lzunja</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>A Pride rainbow? In July? It's more likely than you think 😂</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzunja</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1lzuj4s</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>My sad day of purchase failures</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzuj4s/my_sad_day_of_purchase_failures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1lzug0f</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>First Tim using gel at home...many issues, many questions</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzug0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1lzu2y3</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>OG Nail Blogs - any lists?</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzu2y3/og_nail_blogs_any_lists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1lztscl</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>First time trying nail art 🥰🥰</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lztscl</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1lzsbme</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>ILNP Illusions Collection ⭐️</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzsbme</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1lzs65n</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>I know, I know….</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzs65n</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1lzrg4z</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Kathleen and co Follow Your Dreams</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t771w6p3cvcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1lzr9es</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Pandemonium 🎇</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/esu0ifsc7vcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1lzr901</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Happy Bastille Day!</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gbup2v7tavcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1lzqqmv</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>New release tomorrow 12pm PT!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzqoxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1lzql9d</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>polish haul from my soon-to-be stepmom</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzql9d</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1lzqd0p</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Berry Naughty</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzqd0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1lzpju7</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>ILNP Ballet Slippers to make my gel break more enjoyable</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hvsbfyxkzucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1lzpdls</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>A (probably impossible) search</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xh9y1bneyucf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1lzozph</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Polish &amp; Beauty Expo 2025</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzozph/polish_beauty_expo_2025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1lzokn4</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Indigo Bananas This Shift is Bananas. Unicorn Pee pigment: pictures, thoughts, and feelings.</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzokn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1lzo1lo</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Tibberz makes my nubbies look longer</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzo1lo</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1lznhsd</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Glass bead with Cirque Blue Velvet</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ccm2y66wjucf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1lzmio5</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>You can tell I'm a lacquerista based on the alchemy lab I keep at my desk</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/153i42z9eucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1lzmacp</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Anyone have this dirt trapped in top coat problem? Or Solutions😅</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzmacp</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1lzm84l</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Calcifer🔥</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzm84l</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1lzlxex</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Updated List for Texas Flood Relief Charity Polishes</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fe75i2n9ucf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1lzjem9</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails: Purple Moon - Stunning Solar Polish 💜🤍🌕</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zfyzspgsltcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1lzjbeu</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>UK destashing?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzjbeu/uk_destashing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1lzif83</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1lzif83/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1lziddk</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>A random pic from Pinterest inspired me</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lziddk</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1lzibe3</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Tried something different 💚🖤</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzibe3</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1m0bfz5</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Are my French tips good? I cant tell if they are technically objectively good french tips lol</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xg7x35teqzcf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1m0978x</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Nail Art or Hardware? 😂 Getting Mixed Reactions on This Set!</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0978x</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1m07wxs</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>She’s ready for the beach 😆</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k53zmdyapycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1m07vme</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Some summer flair!</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m07vme</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1m0711u</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Do your hands always match?</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0711u</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1m05lp4</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Did algea nails for a friend!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m05lp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1m05hdy</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Inspired by the TV show Sopranos 🖤⭐️🦆🩸</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m05hdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1m055ss</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>Fresh work: I loved how this design turned out, what do you think?</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2gcp5ip0ycf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1m04wcv</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Mis uñas 🥹</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m04wcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1m036j7</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>A set that I made some time ago, it should be noted that I am an apprentice. Do you like it?</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de9z9k0wkxcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1m01jve</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>I did these nails today. Do you like them? Would you do them? My client requested it</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3y7gtph88xcf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1m0159k</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>The frog's name is Egbert</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0159k</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1lzyno3</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Gigi inspired gelx</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/111snz0onwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1lzx7p8</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Pink Pony Club nails 🦄</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwzedeeudwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1lzwn9x</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Did myself last summery theme nails</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hyslvuo1awcf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1lzvihe</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>PolyGel Help! sculpting with Polygel</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1lzvihe/polygel_help_sculpting_with_polygel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1lzuy9t</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>🎰🎱🎲</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzuy9t</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1lzu258</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Design wheel*</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j54uuer2tvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1lzrf3w</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Doing the most for hands that type 2 words a day</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z5iclaybvcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1lzpf51</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>MARBLE❤</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q90b5jtmyucf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1lzpadt</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Decided to try out western style</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77txv7ssxucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1lzomyg</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Nail art practice</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzomyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1lzo2o6</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Beach set done by @nails_emmywynn on IG 😍 so obsessed and can’t stop staring at my hands 🐚🦀🌊</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzo2o6</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1lznxnq</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>BLUE AURAA 🌀</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lznxnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1lzm0aq</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>GTA nails!!! Driving me crazy that the ak47 is upside down</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzm0aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1lzkyyz</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>progression of gore core nails from last fall 🧠🦷</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7g90a3qt1ucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1lzku2b</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>forgotten Coraline set i did a few years ago, might recreate it with some improvements 🗝️🐭</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ozkd3mtm0ucf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1lzkrdj</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Nail art by me ✨ | When you can’t pick a mood… you wear them all. 🔥⭐🐾 @beauty.chicnails</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekpf9lkxztcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jul 16 08:13:34 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_20.xlsx
+++ b/data/collected_data/2025_07_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C506"/>
+  <dimension ref="A1:C719"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9035,6 +9035,3627 @@
         </is>
       </c>
     </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1m164ol</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>I 🩷 my new nail tech!</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m164ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1m15dce</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Talkn Bout Talons</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m15dce</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1m14m6c</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>X-ray skull ☠️</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hc7uio8c6df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1m14s4s</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>I love this shade 💜</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ywmvk80e6df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1m14cz3</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Any tips to fix my broken nail?</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lfi139kg96df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1m142pz</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>more sets for some friends of mine !</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m142pz</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1m13ttn</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>The most recent set I did on myself &lt;3</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4e0414rq36df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1m13aun</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Nail help</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m13aun</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1m13iah</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Builder gel feels weird?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m13iah/builder_gel_feels_weird/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1m13dx4</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Acrylate free options?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m13dx4/acrylate_free_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1m13mq1</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>can i put partial press ons, just on my nails tip?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m13mq1/can_i_put_partial_press_ons_just_on_my_nails_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1m12x6u</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Nails keep peeling :(</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m12x6u</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1m13eg2</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>This beautiful set I did on my bestie &lt;3 I loved it so much</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m13eg2</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1m13cj8</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>real nails!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m13cj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1m135qc</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>fun summer set :)</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/21s8ifniw5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1m13384</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Aghast at microplastics</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m13384/aghast_at_microplastics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1m12pdq</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Summer picnic🍓🍰🧺</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkq5has9s5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1m12eef</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Any tools to help pressing deep button?</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m12eef/any_tools_to_help_pressing_deep_button/</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1m127lt</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>How do I measure my nails for press-ons?</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5w3gyrnbn5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1m120nv</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Golden magic numbers.Manifestation set incoming.</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xn6bcd4m5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1m11xe7</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Simple Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12es8l5al5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1m10q88</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Why do my press ons look so odd??</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m10q88</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1m119k5</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>White gel?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m119k5/white_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1m11k22</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>X-ray ! How’d I do?🩻</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwu9fyoxh5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1m11elu</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>Bananails 😎</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yd21wj4ag5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1m10o63</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Little toe with crack(?), split(?). Any advice on what this is and how to fix it? It frequently snags my sock (ouch!).</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl7c8wf9a5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1m10l8u</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Am i still able to get a fill?</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m10l8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1m10dzs</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>ChinaGlaze chips really quickly :(</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m10dzs/chinaglaze_chips_really_quickly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1m103rw</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>How can I take a good picture of these?</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m103rw</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1m0z8od</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>How do i fix my broken toe nail</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/of0iwpmzx4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1m10bb9</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Vegas ready 😏</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwqx2ze675df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1m0zux8</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Spicing up 5below Nails 💅</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/adsedjr935df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1m0zgwi</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>my girl cooked so hard she took photos</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0zgwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1m0zgve</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Tips for adhesion near cuticle.</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0zgve/tips_for_adhesion_near_cuticle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1m0xlmw</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>First pedicure</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0xlmw/first_pedicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1m0xu93</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Sweet &amp; simple summer vibes</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjnkaea8m4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1m0xptp</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>First time doing gel nails for myself. Do they look okay?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0xptp</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1m0xoj8</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Better red shade?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkviif1xk4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1m0xjr4</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Holiday nails 💖💖</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzsx49cwj4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1m0xhnw</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Any idea what these colors are? (DND DC)</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co91derfj4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1m0x8f9</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Builder Gel Lifting At Free Edge</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q7ov1pyeh4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1m0xbag</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>nail biting</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0xbag/nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1m0xa2s</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>My first time trying Cajun Shrimp❤️🦐🌶️🧡</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0uzkewrh4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1m0x94f</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Just found my go to builder base gel</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0x94f</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1m0wwab</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>florals for the summer? groundbreaking.</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/falfi5zse4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1m0whek</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>True or False: Some gel polishes can't be soaked off</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0whek/true_or_false_some_gel_polishes_cant_be_soaked_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1m0wrrz</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>I’ve been loving deep french tips lately</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azy69rmvd4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1m0wlhk</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Aurora - inky dinky</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0wlhk</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1m0usci</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>i travel 2 hours to see my nail tech</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0usci</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1m0vo2w</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Im able to make indents in my shiny gel but not matte gel?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0vo2w/im_able_to_make_indents_in_my_shiny_gel_but_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1m0w19r</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>press on newbie — how do i make semi-transparent/jelly styles look good?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0w19r/press_on_newbie_how_do_i_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1m0vpaa</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Thermal polish</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0vpaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1m0vskr</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>As a short nail girlie I LOVE THIS! Next time a nail tech says they can’t do design on short nails I will show them this photo bc this nail salon never misses.</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d47l9jyf64df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1m0vqzp</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Fill time?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo8k8i7464df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1m0vits</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Twinning with my bestie ✨</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qly0ce5a44df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1m0v6y1</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>I didn't expect it to turn out like this!!! I LOVE THE RESULT🥲💕</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0q6pztgs14df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1m0up8k</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>I took advantage of my work vacation and asked for it as long as possible hahaha</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f65yiaw7y3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1m0uk95</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Cat eye gel! Where to start?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0uk95/cat_eye_gel_where_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1m0uei9</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0uei9</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1m0u7f9</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Made something fun today)</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5jin5dpu3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1m0sr5g</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Coffin shape to stiletto is it possible?</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0sr5g/coffin_shape_to_stiletto_is_it_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1m0sm1n</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>The usual or TAP?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0sm1n/the_usual_or_tap/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1m0sh76</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>I love my new nails!😻</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/271grr3ni3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1m0s50n</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Soo, my new nail tech</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psr69qugg3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1m0s1vt</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Cat eye 😍</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0s1vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1m0ritu</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Little nail hack</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zl6js9cc3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1m0rmuv</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>koi fish 🎏</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkyjdkb3d3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1m0rs1o</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>French Nail Design Ideas?</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv1kzvg1e3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1m0rf6z</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Fresh nails wrapped around a refreshment. Stay hydrated</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4xjs3lob3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1m0r3gh</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>New Nails with Heena!!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ifz9hdi93df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1m0q6t3</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>All my nails have different shapes and I am Bad at filing</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg769rqe33df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1m0q431</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>If you're a 90's kid and loved SATION's Cotton Candy nail polish...</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0q431/if_youre_a_90s_kid_and_loved_sations_cotton_candy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1m0py39</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>My cherries 🍒</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wypog6v13df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1m0pitm</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Broke nail by putting on pants. Let this be a lesson: don’t wear pants</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zo4kkwy0z2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1m0pgsr</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>idk what to call these but nail tech ate</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0pgsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1m0pcjv</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Subtle designs? I don’t know her.</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i4qysfuux2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1m0h08t</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Are there any good at home builder gels which work for long nails?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/195k4g6cc1df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1m0gzrn</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>No chip changed colors no</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0gzrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1m0k7cg</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>First time doing my nails</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0i19oaqnz1df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1m0kjzw</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Trying to get press on nails for my trip and need help</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0kjzw/trying_to_get_press_on_nails_for_my_trip_and_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1m0ovzk</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Mani/pedi</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0ovzk/manipedi/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1m0bm1w</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Experience with regrown nails</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0bm1w/experience_with_regrown_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1m0h88y</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>I am a beginner</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kazfdk2e1df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1m0kwo6</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Damage Update</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0kwo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1m0ohjc</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>New nails!! Very happy with how they turned out.</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0ohjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1m0npur</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Nail had super thick growth when I injured my thumb</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0npur</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1m0o5n2</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Im absolutely obsessed</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0o5n2</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1m0o16w</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Barely there glitter - OPI gel Sweet Salty Nothings</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goj0f2u5p2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1m0nxqu</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>first mani in forever</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0nxqu</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1m0l4ce</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>press on nail removal?</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0l4ce/press_on_nail_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1m0mzsw</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Which shape would be good for my nails?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vd0ravjbi2df1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1m0moca</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Nail artist SUPER-GLUED my tips… how to i take them off without damaging the natural nail underneath? (which BTW SHE drilled without asking “bc natural nails are dirty and u dont need em” smhhhh)</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0moca/nail_artist_superglued_my_tips_how_to_i_take_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1m0mgsg</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Press on nail tips</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m0mgsg/press_on_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1m0jjdp</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>Need some help with picking next set</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0jjdp</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1m0m8oa</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>French with a purple accent</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38b1nikbd2df1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1m0lnbd</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Glitter Reef 🪸</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77x2ce8g92df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1m0lf6a</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>I love opals that aren’t pure white. 🥰</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0lf6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1m0l5cu</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Summer cherry blossoms.</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0l5cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1m0kuz8</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Ocean nails🌊🦀</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3xg3rfs242df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1m0k8lu</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>My nails have finally grown!</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxo7qowvz1df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1m16xnx</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>can’t stop staring at them</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0vj3r1vf27df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1m16o46</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Okay, my magnet-obsessed friends. What magnet(s) should I buy??</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/21nvxj6dx6df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1m15osg</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>How long did it take to get fast at painting your nails?</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m15osg/how_long_did_it_take_to_get_fast_at_painting_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1m153g7</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Multi Chrome cat</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/81y74l5dh6df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1m13t7i</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Any recs for rainbowy toppers?</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m13t7i/any_recs_for_rainbowy_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1m1361e</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Skye 🌫️</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m11wfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1m13000</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Vibrant Vinyls Double Bond and leukonychia (white spots on nails)</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m13000/vibrant_vinyls_double_bond_and_leukonychia_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1m12b1s</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Red pikmin nails!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y3i9vkoo5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1m128mn</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Haul Swatch Fest</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pztax8sxn5df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1m11yln</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Is this a skittle?</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m11yln</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1m11u3b</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>I know most QDTCs are applied right after polish, but SH says 2 minutes and I am confused</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/09ue02y3k5df1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1m11iba</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>thinking about this diva, i bet she can give herself a mean mani</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eapzpmlih5df1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1m110pg</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer Strategy</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m110pg/bees_knees_lacquer_strategy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1m10vag</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zon5xwyb5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1m10upw</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>I've got an idea and hear me out...</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65l3pn3ub5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1m10fxt</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Polish – Wiener Circle (PBE 2025 Exclusive)</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m10fxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1m106dp</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Day 2 to Day 10</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m106dp</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1m105wf</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Does anyone know of a dupe for China Glaze - I Have A Blue Attitude or these two colours?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m105wf/does_anyone_know_of_a_dupe_for_china_glaze_i_have/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1m0zksb</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Green halo</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lfxid0hu05df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1m0z2rw</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>How should I shape my nails?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0z2rw</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1m0yvbx</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Cool-toned pink and a lil’ glitter!</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0yvbx</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1m0yajp</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce Polish – Chi Town Blues (PBE 2025 Exclusive)</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0yajp</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1m0y341</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Oil Slick</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zgt6unp5o4df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1m0xydo</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Favorite studio color for under jellies to make them more opaque?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0xydo/favorite_studio_color_for_under_jellies_to_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1m0xl4f</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>She’s so sparkly</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yong5gl6k4df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1m0wp4m</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>recently dived into the world of press ons!!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nnbqhq8bd4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1m0vyvb</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>pomegranates ❤️</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dlzid6kq74df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1m0vuhs</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>DIY jelly</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0vuhs/diy_jelly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1m0vp31</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Fruit nails!</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sy2hfhfp54df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1m0vn6q</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>La Tomatina🍅♥️</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0vn6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1m0vkg5</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Orly Pink Raspberry</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0vd0b</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1m0vggp</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Twinning with my bestie ✨</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fo8z1s1r34df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1m0vbod</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Amethyst dreams</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0vbod</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1m0u3ni</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>💥🫧INLP Hypnosis🛸🔮</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5lwq1iixt3df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1m0twi4</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Any good dupes for Ethereal Mercury?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0twi4/any_good_dupes_for_ethereal_mercury/</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1m0te1z</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>OPI Mystery polish</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j3kudd6zo3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1m0t2mg</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>BKL Haul #1</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0t2mg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1m0t010</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Definitely my new favorite shade of blue...purple...blurple?</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0t010</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1m0swiq</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>A foray into neons with Atomic Polish!</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ijqbtl5dl3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1m0srj0</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>ISO Brick/Ochre Red</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0srj0/iso_brickochre_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1m0sr50</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>What are your favorite monthly (or otherwise) nail polish drops (like PPU and HHC)? I know there’s others out there!</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0sr50/what_are_your_favorite_monthly_or_otherwise_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1m0rmxx</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Texas Charity Polish is live + 25% off everything!</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0rmxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1m0rcaz</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Making regular polish magnetic?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0rcaz/making_regular_polish_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1m0r89h</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>I am now addicted to swatching and labeling</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5z9ngl2ea3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1m0r4ba</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Gel polish brand with least allergy issues?</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0r4ba/gel_polish_brand_with_least_allergy_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1m0qq3k</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>First ever velvet mani 💅</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n3n6iu6273df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1m0n40q</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>learn from my mistake and don’t add nail polish thinner to nailtiques formula 2!</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrude9z3j2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1m0nq6s</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Colores de Carol vs Vibrant Scents Glitter Smoothing Top Coat?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0nq6s/colores_de_carol_vs_vibrant_scents_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1m0q07p</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>First attempt at soap nails and squoval</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0q07p</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1m0py54</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Vixxxen</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0py54</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1m0pjkf</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>This color was made for the glass bead technique!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ju36du4z2df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1m0ph0q</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Do you all worry about getting that spot?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbixdveoy2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1m0pcj9</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Immediate add to cart</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0pcj9/immediate_add_to_cart/</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1m0pcex</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>House Of Hades - My Current Summer Favorite</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0pcex</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1m0p3nc</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Recommendations for polishes similar to Alchemy Lacquer's Emotional Support Taco</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0p3nc/recommendations_for_polishes_similar_to_alchemy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1m0p1ai</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>An attempt to dupe Stumped</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0p1ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1m0oz8b</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Mooncat Heavenmetal</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0oz8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1m0oa9u</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Polished for Days Cosmic Energy</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/am37cwjiq2df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1m0o4u4</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>My firsr ILNP polish! 🥰</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tztzopcsp2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1m0nwnf</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Getting comfortable with natural nails</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/52hdibxbo2df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1m0nesi</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Still Summerin</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ounx2wi0l2df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1m0nehb</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Nail Station upgrade!</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0nehb</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1m0mlop</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Old Timey Nail Care Hints (scroll)</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0mlop</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1m0m7s6</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>shade and stamping plate suggestions for Corelle Lazy Daisy nails?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0m7s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1m0m3ga</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>How can you tell when the next LynB designs sale is?</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0m3ga/how_can_you_tell_when_the_next_lynb_designs_sale/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1m0l6or</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Newbie to magnetics</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0l6or/newbie_to_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1m0kufh</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Anyone else's cat obsessed w jojoba oil?</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0kufh</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1m0kl4q</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>my white whale mani: gemstone nails</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0kl4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1m0k90l</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>I was labeling my swatch sticks and they looked so pretty with the flowers!</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0k90l</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1m0jvbo</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>My office essentials 💅</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0jvbo</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1m0jgrr</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>press on removal?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m0jgrr/press_on_removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1m0j9j3</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Goth sand crabs</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0j9j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1m0ijdw</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Charmed Life (velvet) KBShimmer</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a0cshqnyn1df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1m0iffs</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>I love Emily de Molly polishes</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0iffs</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1m0hywd</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>got some pretty little ILNP neuties to show ya!</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0hywd</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1m0hqhw</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>I discovered that I love pink polishes now</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0hqhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1m0feah</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>My summer staple</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wq6pfxezx0df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1m0d9g1</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Dupes for BKL’s Feo Fuerte y Formal?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0d9g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1m16y9p</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Nail art and a seven year old</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m16y9p/nail_art_and_a_seven_year_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1m16sxt</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>look my New Summer nails 💖💗🥰💞</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m16sxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1m14of6</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Skull x-ray ☠️ do you like the Mohawk? Lol</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pimd0e1xc6df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1m136wo</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>They're not perfect but I really like them.</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw5k4j3uw5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1m12hsh</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>FRUIT NAILS! Part 2, complete set.</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m12hsh</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1m12bed</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Seriously, how many ways can we rock cat eye nails? There’s always a fresh new technique to try.</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/56vqslfro5df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1m1274q</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>I just made these</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1274q</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1m11wxs</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>With or without the red stripe?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m11wxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1m11wj3</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I really like these nails! What do you think?</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cv6793uzk5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1m11if9</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Chest x-ray 🩻 How’d I do?</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgtfbsjjh5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1m116ex</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>PSA to all the girlies. Acrylic paint is the secret to detailed nail art that people pay hundreds for. NO GATEKEEPING.</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecqhsv2oe5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1m11619</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Gel nails at home</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m11619</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1m10njy</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>BLOOMING GEL HELP</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hz2j2ja4a5df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1m10fxz</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>FRUIT NAILS! Part 1</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m10fxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1m0ystc</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Nail art on natural short nails</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0ystc</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1m0yl1s</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3fwgxmcs4df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1m0wsz3</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>A few of my favorites.</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0wsz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1m0w6h4</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Water marble nails</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fln8m29d94df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1m0vkof</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>night themed nails :3</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0vkof</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1m0tyo3</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>I have been trying to learn how to make press ons here is what I have so far</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0tyo3</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1m0rjug</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Cloud nails</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6fuqi0jc3df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1m0o77n</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Polka dots🎀</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e72ool28q2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1m0mbdq</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>First time trying blooming gel</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxa7t2rpd2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1lzzn92</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Doing more nail art on myself! Please don’t be harsh, not looking for advice, I’m showing off cause I’m proud.</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/whkv1exhuwcf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1m0lw7e</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Birthday set for a friend of mine:)</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5r5jfua2b2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1m0ltav</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Charcuterie board press ons🧀🍓🍇</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jxugn46ja2df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1m0lj0n</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Opal nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0lj0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1m0jizc</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>I think it's the most beautiful color in the world! Don't you think?</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6073iiwu1df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1m0j5en</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>they remind me of an overripe banana 👁️👄👁️</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0j5en</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1m0ionr</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Nail supply store recs from Lazada/Shopee?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m0ionr/nail_supply_store_recs_from_lazadashopee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1m0h29o</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Summer nails 🫐🍋🐟⭐️</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0h29o</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1m0gr3g</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>I love doing these types of designs, even though they are simple, they make the nails look great and make them look very subtle.</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9fykmb2a1df1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1m0g913</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Tried to do some cute nails</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0g913</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1m0eh0h</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Did these to go to a festival 🌈</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m0eh0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1lzmgwi</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Rate 1-10 🌟</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1lzmgwi</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jul 17 08:13:36 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_20.xlsx
+++ b/data/collected_data/2025_07_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C719"/>
+  <dimension ref="A1:C928"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12656,6 +12656,3559 @@
         </is>
       </c>
     </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1m20lia</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Best type of extensions for growing out natural nails.</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m20lia/best_type_of_extensions_for_growing_out_natural/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1m203gg</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>can I fix this gradient at home?</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m203gg</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1m21p89</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>I Know They Are Gonna Break 🥹</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y39oisww5edf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1m21g3n</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Marble and snakes</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl4g6u1x2edf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1m219vc</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Spilled nail Polish remover on fresh set</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m219vc/spilled_nail_polish_remover_on_fresh_set/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1m20t0f</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Nail polish break, so that my nails can recover a bit😍 💅🏽</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m20t0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1m20fr2</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Jade nails</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4wfg68crddf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1m1zoo4</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>press on etsy stores</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1zoo4/press_on_etsy_stores/</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1m1zjej</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Never had my nails professionally done, where should I start?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvozgm3jgddf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1m1z811</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>First ever time doing extensions and gel at home…</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1z811</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1m1z41c</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Need Recommendations: Short Term Nail Need</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1z41c</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1m1z3i1</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>May every evil eye in your life go blind 🧿 🪬 ⭐️ 🧡</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaujhx2ycddf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1m1y8lp</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Press-on Nail Removal</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kg8iz5m94ddf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1m1xuf3</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I made my own press on nails 😊</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1xuf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1m1xsao</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Dark knuckles due to UV lamp?</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1xsao</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1m1xp27</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>In my aura era 🪐🧚🏼‍♀️💜🍊</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1xp27</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1m1xbdr</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Classic Red Pedicure</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35qafdogvcdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1m1xaur</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>My nails from the past few months</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1xaur</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1m1x7xw</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>First time trying out clay sculpting gel!</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1x7xw</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1m1wr2n</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Glow in the dark</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1wr2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1m1wqry</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Let’s go to the beach 🏝️</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7j1u8f7qcdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1m1u9ct</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Hi all!! (Again) I’m getting married in November and I need help finding nail designs ! Here is my wedding dress for inspo, I’m open to anything. :)</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ty52jsq4cdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1m1w2as</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>First and last time getting French toes</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d96qxu74kcdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1m1v9ge</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>What my client asked me for today! SO CUTE, RIGHT? 🥹🥹🥹</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8n039v8dcdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1m1v4m3</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Questions</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1v4m3/questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1m1u3yq</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Marbled nails</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gtk2stf3cdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1m1twwq</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Love my new nail stickers</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cws9y1w1cdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1m1tmjp</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>What is everyone’s favorite double sided tape for displaying press on nails?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1tmjp/what_is_everyones_favorite_double_sided_tape_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1m1tpg4</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>I’ve wanted this design forever.</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1tpg4</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1m1tmea</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Does anyone still appreciate a beautiful red manicure</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pc7qry9zbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1m1tcjg</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>My favorite set!</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1tcjg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1m1t0jc</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Polygel fill a bad idea?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1t0jc</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1m1sz6l</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>I liked them.</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/azdur8wxtbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1m1swt9</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1swt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1m1rtzh</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>My nails keep splitting down the middle :(</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yq37wpmukbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1m1ss53</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Latest set 🔥🧊🔥</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1ss53</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1m1sqe3</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Is it normal for builder gel to look this thick?</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1sqe3</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1m1slmv</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>silver daggers but make it sparkly</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dp6do9vqbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1m1sis0</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I noticed these deep wavy lines on my nails but I don’t know how it happened pls help</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1sis0</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1m1sg80</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Acrylic refill…should I complain?</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1sg80</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1m1ru83</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>my fingers are crusty rn but love these press on nails !! @lilynailsart.co on ig! 🌊🪸🐚🐬🫧</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1ru83</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1m1sfni</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>First time trying blooming gel.👀</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qu0oiiijpbdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1m1s5e1</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>What shape should I be asking for? I asked for almond but these seem very thick and fat.</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1s5e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1m1rvmk</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Red nails always hit. 😌</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqxv5ch7lbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1m1qwij</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>My nails are so short/small that “ultra short coffins” are too long for me</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qimdllirdbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1m1qvfc</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>My daughter wanted me to get blue sprinkles for her birthday</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vh035egjdbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1m1qtm5</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Had time off work go this long set</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1qtm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1m1qt8l</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Obsesseddd</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sj9p5ii2dbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1m1qsgl</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Opi - angel flight to starry nights</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1qsgl</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1m1q4m8</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Speaking of icy nails…</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zc2vrzc18bdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1m1q313</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Nails as icy as the Northen Sea🧊</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ukp5qxp7bdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1m1ocyu</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Lemon french tips for Summer by my Nail Tech 🍋</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsi20bfevadf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1m1o72x</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>stop gel x from popping off</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1o72x/stop_gel_x_from_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1m1mx2c</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>how do I help nail growth?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nz89fbcladf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1m1o42d</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Sticky top coat</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8w3ln41ntadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1m1m45n</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>How do I better blend the old builder gel with new?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vc2k7gpfadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1m1n6i3</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>How tf do I ask for a Gel X fill in?</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1n6i3/how_tf_do_i_ask_for_a_gel_x_fill_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1m1nec3</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I rarely get manicures but holy I love this colour/shape!</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tngvfqznoadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1m1mfe0</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Holo rainbow🌈✨💅🏼</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2isnvyuhadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1m1lzi7</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Best shape for my nails?</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xi95pk1ueadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1m1ltub</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Japanese gel popped off- brown underneath</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ans6qvnudadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1m1lsxt</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>How to care for broken nail exposing skin underneath?</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx4ndbqodadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1m1lnfi</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>ILNP - Frankie</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ah933s6ocadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1m1kt32</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>before / after</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1kt32</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1m1kseq</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>🦀💙♋️Unintentional Cancer Season Nails.</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1kseq</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1m1ksc9</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I’m obsessed. 🩵</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/clarqv007adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1m1kkln</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Neat Pink Cat Eye Nails</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1kkln</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1m1ki3g</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>My favorite set of this year 🤍 my x</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/294heqb25adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1m1kf04</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Peaking Mountains with my Birthday Mani ✨⛰️</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klzb64hh4adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1m1kch1</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cocnrd904adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1m1kbog</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>classic french tip nails</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kggg47zu3adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1m1k3wz</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Catching butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5v37633f2adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1m1juxe</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Frog and flower nails 🐸🌼🥰</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1juxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1m1jsa9</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Random summer theme 🌞</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1jsa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1m1js1f</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Always love a clean ombré look</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9msszp70adf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1m1jlcz</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Purple Cat Eye 💜</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tdm5k271z9df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1m195ie</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Feeling Discouraged</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m195ie/feeling_discouraged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1m1cl24</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>To Cut or Not to Cut?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1cl24</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1m1iuvm</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Nails I did recently. Rate my work.</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1iuvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1m1i3tw</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>New nails 🍒</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsap2e67p9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1m1hqz4</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>new nails!</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1hqz4</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1m1hodc</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>just admiring</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1hodc</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1m1hj86</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>My floral collection 🌸💅</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnzqrarfl9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1m1hi4w</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>New nails! In love with them</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu37ks18l9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1m1hce0</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Sheer pink with a hint of sparkle 💗✨</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnhvfzf4k9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1m1fvdm</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>What do I do with the numbers on the bottom of fake nails? Does everyone file them off or just leave them?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1fvdm/what_do_i_do_with_the_numbers_on_the_bottom_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1m1c2hf</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>first press on nails</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dzup1ofyi8df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1m1gywc</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Just a curiosity</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib4qiu1mh9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1m1gtj1</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>When life gives you lemons 🍋</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1gtj1</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1m1frl5</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>💅</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1frl5</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1m1fiip</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Pastel chrome swirly something</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1fiip</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1m1fane</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>How much would you charge/think you would be charged for this nail set?</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1fane</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1m1f33o</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>HELP gel x application</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/10k2xlq359df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1m1ehzt</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>First time getting my nails done!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kkxnrq7519df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1m1efbk</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>I'm a 54yr old male, straight. This is my third different design since I started getting my nails 💅</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1efbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1m1e6bb</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Understanding what I’m doing wrong</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1e6bb/understanding_what_im_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1m1e0pk</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>My first set with magnets and dual forms!</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n66gkjnrx8df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1m1dtng</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Who does it better?: Nail tech with their nails done or not done</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m1dtng/who_does_it_better_nail_tech_with_their_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1m1dldw</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Over growth of keratin?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i0f17i2ou8df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1m1dkmu</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>First time not getting a pink/nude set!</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k94xs35ju8df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1m1zunr</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Regular Polish Brand Recs</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1zunr/regular_polish_brand_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1m1xn7k</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Does this look like a 70 lbs magnet job to you?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dg4w4cjiycdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1m1wn24</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Hello, I'm new + a question or 2</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1wn24/hello_im_new_a_question_or_2/</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1m1wlcw</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>PBE Exclusive] 🏈 Sassy Sauce Polish – “Touchdown” (blue-to-orange thermal)</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1wlcw</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1m1wj74</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>wedding manicure ✨</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hq1e9yaocdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1m1wae1</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>comfort polish lol</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1wae1</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1m1w3mu</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>KB Shimmer Get Your Knit Together</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/k17aam68kcdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1m1vyha</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>Manimod drawer inserts?</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1vyha/manimod_drawer_inserts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1m1vqj1</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Would you ever intentionally dupe yourself because the polish was a different brand?</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1vqj1/would_you_ever_intentionally_dupe_yourself/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1m1v93l</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Polishes with Flower Power from ILNP vibes?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1v93l/polishes_with_flower_power_from_ilnp_vibes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1m1v8v8</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>First magnetic polish</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y4rfvlv3dcdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1m1v8sm</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Chopped my nails down on accident😭</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4j81rwvjccdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1m1ttf8</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>brightest polish i’ve ever worn ✨</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1ttf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1m1tsei</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Proving that yellow polish CAN look good on non-warm skintones! (2 pics per shade - 9 shades)</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1tsei</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1m1trek</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m16ax0</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1m1thcx</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>I Hate to Say It…</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1thcx/i_hate_to_say_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1m1t7rs</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Show Me Your Favorite GREEN Polish</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1om2deazvbdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1m1st54</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>I know everyone is into magnetics (can't wait to get some), but can we appreciate some holographics?</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hc7sq9dlsbdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1m1sj2m</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>RIP Shadow Daddy (and my carpet)</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbx29kkaqbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1m1sfzi</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Blues like this?</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/039xd3ampbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1m1s75r</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Summer Fun-sies to the Rescue!</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1s75r</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1m1rzwh</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>ILNP - Moonlit 👻</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1rzwh</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1m1rwbd</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Loving this combo!!</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3dldpcxclbdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1m1ri6w</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Lacquer Set Recommendations</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1ri6w/lacquer_set_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1m1r7we</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>My first experience with holographic glitter polish 💿🪩📀</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b99rrab4gbdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1m1qt91</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Gel top coat that glows</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1qt91/gel_top_coat_that_glows/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1m1qrwy</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>My phone camera sucks so this isn't the true color, but: "Cleopatra" from Dollar Tree with Electric Carnival ILNP topper. Don't sleep on Dollar Tree polish y'all!</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1qrwy</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1m1qho4</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Anyone else struggle to wear their favorite DD/LE polishes without feeling like you're wasting them?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1qho4</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1m1ppxo</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>What a time to be alive</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqoa48f35bdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1m1phvz</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Fishing Lure Nails!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as53ye0h3bdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1m1p7tz</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Can I get feedback on my shaping? Are these Round or Almond?</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1p7tz</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1m1p0bu</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Dazzle Dry -different top coat</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ytndggvyzadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1m1omz0</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Lurid- Our Laughter Carries on a Warm Wind</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1omz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1m1omhy</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Feeling stuck and not sure how to proceed</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1lvhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1m1oke5</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>InspiredSense order arrived!</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ws7wm3uwadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1m1o3nv</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>First time twirling magnet</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1o2bx</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1m1o070</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Do you add a regular top coat PLUS a quick dry top coat?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1o070/do_you_add_a_regular_top_coat_plus_a_quick_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1m1nwt1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Sassy Sauce and Jen &amp; Berries</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1nwt1</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1m1nn3v</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Should I do my other hand or do something else? Lol</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1nn3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1m1ncm5</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Semi sheer look without using gel?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9rn66ysboadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1m1n65x</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Another day another magnet</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etm0lyw2nadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1m1n5q6</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>house of hades never disappoints 💅</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1n5q6</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1m1mmz3</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>A/B testing thick and thin layers of regular topcoat</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1mmz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1m1m9zp</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Disappointing Magnetics?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p3se2oxrgadf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1m1m6w7</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Tried to give my chipped nail the landlord special but it's a thermal polish and now the colors don't match 🤡</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pk14gwj7gadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1m1m33t</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Ice cream sprinkles</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6u8epxthfadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1m1lrt5</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>My first magnetic polish</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wz9f2o0hdadf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1m1lnor</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>ILNP - Frankie</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnb8tdwpcadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1m1lcrh</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>feeling blue</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1lcrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1m1l1pn</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Emily de Molly: Eternal forces</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1l1pn</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1m1ky6d</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>How to magnetics?</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1ky6d/how_to_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1m1kqvj</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Halo practice</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l4jzjctp6adf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1m1kbg9</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>🍇💜 Cassiopeia 💜🍇</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1kbg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1m1jfi0</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Do indie or drugstore nail polishes last longer without chipping?</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1jfi0/do_indie_or_drugstore_nail_polishes_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1m1j7c3</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Submitted for the consideration of the Magnet Society... 🌌🧲</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/blxlrwjyv9df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1m1iz9w</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Its no fancy magnetic but Wished for Tomorrow catches the light above my kitchen sink pretty fantastically ✨️</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wrth8zjwu9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1m1iwzf</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Too thin a coat of topcoat may be why your mani does not last</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1iwzf/too_thin_a_coat_of_topcoat_may_be_why_your_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1m1ir13</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Y’all don’t make fun of me but…</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1ir13/yall_dont_make_fun_of_me_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1m1hy32</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Favourite silver nail polish?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1hy32/favourite_silver_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1m1hum7</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Mooncat Velvet Rose vs ILNP Sugar Plum ???</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1hum7/mooncat_velvet_rose_vs_ilnp_sugar_plum/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1m1hshz</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Nail vinyl help</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1hshz/nail_vinyl_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1m1hogq</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Is this the answer to my acrylic allergies?!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cxd9p7oem9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1m1hnm4</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>so are we still doing unhinged magnet setups around here or</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ir23exl8m9df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1m1hl1k</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>My glass bead set up</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1hl1k</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1m1h9kx</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Successful(ish) Glass Bead</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/38yuhoslj9df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1m1guvu</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Nail art stamps and nail molding, and glue questions</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1guvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1m1fn17</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>So Happy With This Combo!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1fn17</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1m1fgb6</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I think my sunscreen went through my top coat and made my nail polish fade</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1fgb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1m1fcpy</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>OPI Russian Navy Alternative</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1fcpy/opi_russian_navy_alternative/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1m1f94f</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>"Heavy duty" cruelty-free Top Coat recommendations</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1f94f/heavy_duty_crueltyfree_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1m1ejf4</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I'm curious: why do you prefer regular nail polishes to gel polishes?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1ejf4/im_curious_why_do_you_prefer_regular_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1m1e65q</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>My 28th birthday nails!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1e5r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1m1dbgr</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>do you like glowy blurple nail polish &amp; cute cats? yeah, me too 🤗</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/d6bobf4as8df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1m1cfnj</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Okay you genius magnet freaks, I get it!! (BKL By the Light of the Moon)</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1cfnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1m1ceb4</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>are these ai</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dzf6ctkl8df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1m1cbcx</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Lightwave by ILNP 💟✨</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vzco1q9xk8df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1m1bfh7</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Help me find a ridiculously overly specific shade of pink please? (See comments)</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1bfh7</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1m1bd4u</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Baby’s first bee’s knees!!!</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mc9nuqx6d8df1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1m1aif2</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>How long does your regular polish last?</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1aif2/how_long_does_your_regular_polish_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1m1a5kv</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Opi nail envy original ???</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1a5kv</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1m19tvy</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Applying regular gel over one step gel polish?</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m19tvy/applying_regular_gel_over_one_step_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1m19bbi</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Looking for a specific color polish</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m19bbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1m197ez</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>When in doubt, go green!</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m197ez</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1m18ry2</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Looking for an alternative to "Genius in the Bottle" by Catrice</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m18ry2/looking_for_an_alternative_to_genius_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1m18ear</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Which one is better?</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5rc7i3uj7df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1m20pzz</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Mothman and SCP Scarlet King Nails</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m20pzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1m1yaqe</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Who would wear these? 😚</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l81vhmkv4ddf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1m1x990</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Amando mis uñitas 😍</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qig5idkuucdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1m1x2ut</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Algae and fish nails I did for friends!</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1x2ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1m1umms</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Beginner diy nail art</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foccigxv7cdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1m1thzb</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Is anyone else patiently waiting for Spooky Season? 👻</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lt1v3a1dybdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1m1shes</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>First time making a set (WIP)</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62uu91gxpbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1m1sdx0</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>First time using blooming gel.👀</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rojz5706pbdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1m1s7vg</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Tiger and bird from kpop demon hunters!</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o0w3mrttnbdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1m1s7p2</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>New press on nail set I made!</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjkbur7snbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1m1s0ge</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>I want a hotdog real bad</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1s0ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1m1re5w</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Titanic inspired nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a6aa18ighbdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1m1pmdv</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>I made my nails into keychains 🙈</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1pmdv</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1m1ny88</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Any tips on how I can make the flowers pop more?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96rfbu5jsadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1m1ne4z</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Summer Time Girl 🪸</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9g68wpmoadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1m1mt1p</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Project for Paul Mitchell the nail school</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1mt1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1m1lb2j</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>To add a glitter ‘scale’ or two to each nail (like The Rainbow Fish) or leave em be?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsy3eogfaadf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1m1jb4a</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>sets i did for friends !</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1jb4a</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1m1ifqh</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>First ever nails I’ve made!</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71a7r0y2r9df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1m1h8ys</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Pastel chrome swirly something</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1h8ys</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1m1gxwq</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Summer jungle nails!</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1gxwq</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1m1e5r1</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>My 28th birthday nails!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1e5r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1m1ce93</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>By the Seashore</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywohkjbkl8df1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1m1bwkn</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>katseye music video inspired nail art</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m1bwkn</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jul 18 08:13:29 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_20.xlsx
+++ b/data/collected_data/2025_07_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C928"/>
+  <dimension ref="A1:C1119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16209,6 +16209,3253 @@
         </is>
       </c>
     </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1m2wgi7</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>natural nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2wgi7</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1m2siu3</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Products</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2siu3/products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1m2up3b</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>I did my thesis presentation / graduation Nails</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15tva0b1rkdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1m2ugq9</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>Tiny Daisy Nails🌼💅</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jx6anh0dokdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1m2sn3r</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Stopping biab - advice on press ons? Stickers?</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2sn3r/stopping_biab_advice_on_press_ons_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1m2sknx</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2sknx</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1m2sa7z</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>MY FAVORITE SET EVER</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23i8yzqp2kdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1m2s04e</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>gel x glue help</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2s04e/gel_x_glue_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1m2s017</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Second attempt at gelX… (repost)</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2s017</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1m2rsl6</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Opinions: Best Gel for Sidewall cracking</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2rsl6/opinions_best_gel_for_sidewall_cracking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1m2rp9y</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Being able to do my own nails is such a game changer</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z4ykxjw8xjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1m2rhuo</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Shark week oo ah ah</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14xj0bjdvjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1m2rbv2</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Vacation nails!</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zykvj2gwtjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1m2r5lk</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>fresh set!</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2nofk4ddsjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1m2qlbu</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>💜💅</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2qlbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1m2q7ay</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Shark week</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2q7ay</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1m2q2la</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>nail embodiment of the raining tacos song</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xz2608ivijdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1m2ppvb</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>my birthday nails gave me lifeee</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ppvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1m2pj9i</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>DIY acrylics</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2pj9i/diy_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1m2pa9q</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/di42rs12cjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1m2okc7</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>first time getting my nails done in a long time and i’m so happy with them 💕</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uk0viiyv5jdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1m2ofx5</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Nails of a Scorpio ♏️ 😆</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8xa0rgtu4jdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1m2o7jb</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Moms - how are we unbuckling car seats with long nails?</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2o7jb/moms_how_are_we_unbuckling_car_seats_with_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1m2o77q</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Stars are hard to do</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2o77q</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1m2o3sr</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>I can’t wait for fall! Getting ideas ready!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sexasm0y1jdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1m2nr2x</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>After my somewhat failed attempt at painting Rumi I tried again with Zoey! Just serving face right now but tomorrow she will be finished 💞💞</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4exlyk84zidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1m2nnch</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>I'm a newer nail artist,  but I did these press-ons recently :)</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9zk8nq6yidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1m2mcla</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Catrice sheer beauties+questions</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otqb9twsnidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1m2n6pz</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Nails for the weekend</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ec4ailjuidf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1m2mx4f</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>advice and or feedback</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2mx4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1m2mrsb</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Thoughts?</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l6xeo444ridf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1m2mhji</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>What shape of nails would suit my hands?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1eyi8gjvoidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1m2m913</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Refusing to let go</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmm1v7l1nidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1m2kmjo</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Summerween nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2kmjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1m2ls6f</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>I love my nails</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpx9q15ijidf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1m2kviy</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>The Very Hungry Caterpillar</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2kviy</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1m2lo6m</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Sally Hansen - that's a blazing</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2lo6m</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1m2lkdv</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Dupe for “Drunk in Public” by Wicked Polish?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5smncrthidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1m2ld0j</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Ladybug nails 🐞</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ld0j</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1m2kmyp</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>At home gel nails… newby who isn’t good</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2kmyp/at_home_gel_nails_newby_who_isnt_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1m2kiy0</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Here I leave you my nail work in Soft gel!!! It's been a long time since I did... what do you think?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2kiy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1m2kd2p</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>what style is this called?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20zaw5dv8idf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1m2k021</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>CHROME POWDER IS JUST MICAH PIGMENT POWDER FOR RESIN</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2k021</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1m2ju2r</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Gel nail</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2ju2r/gel_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1m2jsxa</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Nail Glue</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2jsxa/nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1m2j6w6</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Pride week in my city 🌈💎💖✨</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2j6w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1m2jc4c</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Summer nails</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2jc4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1m2j090</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Did my nails today!</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2j090</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1m2izxv</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>💜 Polished For Days Goblins and Ghoulies 💙 Is it spooky season yet? 👻</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2izxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1m2iye7</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>coraline set done for my friend!!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2iye7</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1m2igbb</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>I went with something different than my usual cats eye this time</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2igbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1m2i2me</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>started doing my own gel nails so i stop picking at my finger skin. getting better!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2i2me</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1m2go53</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Reasons for changing to gel nails as opposed to press-ons?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2go53/reasons_for_changing_to_gel_nails_as_opposed_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1m2hqgm</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Natural nails without nail polish?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2hqgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1m2he1e</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Cat Eye Chrome</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s1yvxll2ohdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1m2hc9i</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Still learning how to do my rubber gel nails at home.</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2hc9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1m2hayn</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Lifelong nail biter, now getting my first professional manicures!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2hayn</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1m2h6qz</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Literally obsessed with my nails!</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ohrj2uonmhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1m2h6k1</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Wild Berry Pop-tart Nails 🫐🍓</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfx59w8lmhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1m2gmws</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>French Tip with Sunflowers</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kr69dxnrihdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1m2gf6w</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Love these!</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2x33rvoahhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1m2g879</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Nails growing in paler</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ccudjiyfhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1m2g03i</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Any recommendations for non gel super shiny glittery polishes?</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2g03i/any_recommendations_for_non_gel_super_shiny/</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1m2fil7</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Crisp pictures</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2fil7</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1m2eapz</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Should I get my Gel-X replaced right now?</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2eapz</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1m2csys</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Does Anyone Know Why This Happens?</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b33l7d0usgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1m2doz8</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Fiberglass nail repair stickers</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2doz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1m2fh4s</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Thanks for the inspo u/noseyandinterested</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2fh4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1m2fs4e</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>We're growing well but these index fingers be like</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2fs4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1m2f8ru</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Gloomy Bear 💅🏻</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3nlv0ia9hdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1m2e1b9</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Birthday nails!!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6yhnsm441hdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1m2d6gs</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Palest baby blue for upcoming birth 🩵👶🏼</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2d6gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1m2d29p</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Blue butterflies 🦋</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2d29p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1m2cs80</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Is this UV gel or normal polish???</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9ypv6ppsgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1m2cr4u</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>How to take good pics</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m2cr4u/how_to_take_good_pics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1m2cdsa</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Favorite french for every day</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2cdsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1m2cdfd</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>✨✨2</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2cdfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1m2c9ue</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>✨✨</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x24dj717pgdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1m25vd5</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>First time getting biogel</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m25vd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1m29lo3</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Birthday Nail Art</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/us92z02v6gdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1m2brmq</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Freshly set done, love the colors</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nfuvjpqllgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1m2blwj</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Idk about this guys…i like blue- but I’m not sure if it’s my colour 🥲</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2blwj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1m2bl1a</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Im a long nailed girlie now?!</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2bl1a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1m2aqf9</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>My nail lady killing it again 💅✨</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzwl8qjnegdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1m2abhj</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Do you ever get post-nail clarity and regret the shape/colour</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osffp8xsbgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1m29wbk</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Set I did on my sister</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjy3ubyw8gdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1m29ff1</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Nail Weakness and Peeling</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m29ff1/nail_weakness_and_peeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1m29cuk</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Essie "eternal optimist" on natural nails</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m29cuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1m28xln</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Dandadan nails 💅🤣 kinda cute</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m28xln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1m28orb</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>got my nails done a week ago but from time to time my nails would feel like it’s tingly/stinging</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qgla81g0gdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1m27mkn</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>How to improve cuticles?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m27mkn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1m27em7</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Acrylic paint stuck under nail</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m27em7/acrylic_paint_stuck_under_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1m279us</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Nails I did today :)</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/978010gwpfdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1m271gd</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Shark week nails</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m271gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1m26cgw</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>My first nails, I'm so happy that I could cry</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/846otg8hifdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1m25xyg</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Should I try a different shape?</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qauusiyefdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1m25p18</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Looking for the glossiest clear coat</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m25p18/looking_for_the_glossiest_clear_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1m254zj</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>My natural nail beds are so small/short that these XXS nails are still too long for me</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v61hgfui7fdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1m24rfq</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Natural nails (+ clear polish) after biting for 20 years. Stopped biting in February (6 months).</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m24rfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1m2405d</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Nail bed (I think ?) changing color</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljzl9hr7wedf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1m2uypj</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Tell me your fave nude polish that's actually opaque 😭</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2uypj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1m2took</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>July is Disability Pride Month!</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2took</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1m2stbn</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Saw this and thought of you all 😘</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rqve5f5o7kdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1m2s7ag</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>by the light of the moon bkl</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8a62b37y1kdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1m2rtrd</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Still trying to find my shade of red</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7en9886fyjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1m2r69f</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Dam Nail Polish Hellfire</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2r69f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1m2qyrr</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>I just can’t resist a polish with a blue glow ✨🩵</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ddmxzwkmqjdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1m2qsm3</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>By Vanessa Molina Sea of Stars PPU June 2025</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2qsm3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1m2p5sc</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>What's the deal with top coats?</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2p5sc/whats_the_deal_with_top_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1m2p2fb</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>dupe for Kafkaesque by Mooncat (super dark brown)</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v38ru917ajdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1m2ogjg</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Window washing vs nail integrity</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2ogjg/window_washing_vs_nail_integrity/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1m2n8iz</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Why does the end of my top coat turn matte</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/518iqz1uuidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1m2n6qx</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Color streaks in Atomic polish creme</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5c5bgpjuidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1m2n18x</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Red delicious!</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2n18x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1m2ms9l</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Finger gems ❤️</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ms9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1m2mi7s</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>E-files &amp; Drill bits</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzdhjuu0pidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1m2mbkr</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>A quiet day at work means nails are painted!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7cphr2lnidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1m2m7r2</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>How to pack collection for long distance move?</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2m7r2/how_to_pack_collection_for_long_distance_move/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1m2ltw0</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>After two days I’m still obsessed!</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/494mk6avjidf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1m2lqqd</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Bad user experience with PPU polish</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2lqqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1m2lf77</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Love a skittle with different finishes!</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2lf77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1m2kj8s</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Purple and teal flakes</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/snau3hp5aidf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1m2kfdx</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Fairy vibes</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u4wpvp7c9idf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1m2johu</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Comparisons for the new Cracked Spirit of Rebellion collection</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2johu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1m2joe3</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Nails peeling from PVB</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2joe3/nails_peeling_from_pvb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1m2jaq8</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Forbidden Fruit glass bead style.</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dgcbbj791idf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1m2j9xy</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Pride week in my city 🌈🤍✨</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2j9xy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1m1p4d0</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>What is the bulb on glass oil pipettes for?</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m1p4d0/what_is_the_bulb_on_glass_oil_pipettes_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1m2hleb</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Lumen Glass Frog (v3) PPU Rewind</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2hleb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1m2ivya</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>💜 Polished For Days Goblins and Ghoulies 💙 Is it spooky season yet? 👻</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ivya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1m2ip7e</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Laqueristas! New magnet drop?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z9sw184xhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1m2i1od</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Pisces the Future</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2i1od</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1m2i0ej</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>De-influence my KB Shimmer shopping cart</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/voiru6kcshdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1m2hw5q</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>1st time ordering from Syzygy - is this normal?</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2hw5q/1st_time_ordering_from_syzygy_is_this_normal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1m2h4pp</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Schneewittchen is THAT red</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2h4pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1m2fu0d</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>summer skittle 🦋💚🍋🩷</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2fu0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1m2fn8g</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Jelly help!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nk2f9n6zbhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1m2ffyt</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Broken Nail Help</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29yaejxfahdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1m2dveh</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>New All BKL Mani</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2dveh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1m2dodt</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Stupid Question: topcoat question : what do you do if you miss your window to apply QDTC?</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2dodt/stupid_question_topcoat_question_what_do_you_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1m2d42r</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Using glitter grabber on nail stickers is a game changer</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwa1fkcgugdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1m2c16r</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>It started with a riot</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xp2himuhngdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1m2bprz</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Today's vibe: ultra feminine picnic princess</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2bprz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1m2az30</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Anyone good at ID for mystery OPI?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2az30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1m2avcf</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Simple French tips</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/thg5zgmlfgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1m2akb6</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>350 total</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qucemcfgdgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1m2af8j</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Ignore the Seche Vite Shrinkage... REEEEED!</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2af8j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1m2acjc</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Love a good prugly sheer!</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2acjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1m2aahu</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Discontinued Polish</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2aahu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1m2a9zu</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Chipping Gel</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fi01j5vhbgdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1m2a6f0</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Can I use a LED gel light on regular UV gel polish?</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2a6f0/can_i_use_a_led_gel_light_on_regular_uv_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1m2a1b2</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Sunset Light</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5hkftvpu9gdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1m2a00j</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Base (and top) coat blues</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2a00j/base_and_top_coat_blues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1m29t0j</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>This is like a better, more shimmery version of Petals for a Narcissist and I'm here for it!</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02jls2ba8gdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1m29brd</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Lurid Joie de Vivre</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m29brd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1m28q4w</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Kitchen sink'd my nails</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrjaft3q0gdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1m28da2</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Introducing: speaker magnet</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m28da2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1m28al8</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Issues with Seche Vite gel effect, what am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3wty5x5pxfdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1m286y8</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Recently found this bag of polishes at a thrift store for $3, so I took a chance on them and I’m not mad about it!</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m286y8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1m27eb9</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Vacation nails</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m27eb9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1m27dt2</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Modeling pretty rocks from my yard with Fata Morgana</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m27dt2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1m2752o</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Bring Me the Amber</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lhut9ycvofdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1m2702p</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>The only polish I got during June PPU was a winner!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py9lv1asnfdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1m26saj</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer to Haunted Polish?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m26saj/ethereal_lacquer_to_haunted_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1m265pe</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>What do you think of essence nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zcl01xbvgfdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1m2620q</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>What the hel-iconia</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2620q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1m25tfb</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Can I use nail polish thinner on glow in the dark polish?</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m25tfb/can_i_use_nail_polish_thinner_on_glow_in_the_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1m224fg</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Can anyone recommend a regular polish in this color? This is a gel polish I had done many years ago at a salon, but unfortunately I don't remember the name.</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ioctbiotaedf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1m2ligb</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Hand-painted ZARA LARSSON NAILS 💅</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ligb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1m2t7zb</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Experiments in chrome powder (first time)</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tin81jaobkdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1m2sjaw</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Carrying these babies is a little long for my liking, but I love this design. What do you think? How did they turn out?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvfnzg915kdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1m2rkrb</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Recently did this set!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gob8onq2wjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1m2qqgs</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Have faith!!</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zcrzmmkojdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1m2q0ju</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>internet nostalgia set !</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vcyuy7eijdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1m2pxx9</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71zb3u2shjdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1m2p83h</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Short manicures that I’ve done!</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2p83h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1m2p0l7</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Freestyle</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xci1m21s9jdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1m2nrby</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>After my somewhat failed attempt at painting Rumi I tried again with Zoey! Just serving face right now but tomorrow she will be finished 💞💞</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ix94yoe6zidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1m2ncwp</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>look Morty im nail rick !!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ncwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1m2n93p</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Art deco nails</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8fmmbd3vidf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1m2ly0m</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>What is missing?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ly0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1m2lfkm</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>New set to match my '07 Dodge Daytona Charger Sub Lime edition no. 548/1500</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2lfkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1m2hrma</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>First attempt with blooming gel. 💜</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2e4vjq5mqhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1m2hmnx</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Feeling Fruity!</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2hmnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1m2h0io</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Me hago sola , pero no me convenció jajajaja ustdes que opinan ?</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0yjy457lhdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1m2fzo4</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Love this result 😍</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l3brzs8cehdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1m298hf</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Shark week nails</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m298hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1m28suo</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>beach nails</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m28suo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1m28bck</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>This my first ever set of nails i tried hows it ? lemme know if u want to do ur nails (did nail tech course)</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m28bck</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1m27227</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Delicadas?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2bdmp316ofdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1m25n8k</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Wild Berry Pop-tart Nails 🫐🍓</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dov40ktbcfdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jul 19 08:11:49 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_20.xlsx
+++ b/data/collected_data/2025_07_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1119"/>
+  <dimension ref="A1:C1320"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19456,6 +19456,3423 @@
         </is>
       </c>
     </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1m3qtma</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>𝑗𝑢𝑠𝑡 𝑚𝑒&amp;𝑚𝑦 ℎ𝑒𝑛𝑛𝑎💋❤️✨</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y5ix296igsdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1m3qiox</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Nail tech wants to charge me another $30 after three nails broke in only 3 days</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3qiox/nail_tech_wants_to_charge_me_another_30_after/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1m3p6lf</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>First time press on experience</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5d6gbrc1yrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1m3ozkk</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>How can I prevent these cuticles from growing back so fast?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydk583bvvrdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1m3nja7</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Porcelain</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3nja7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1m3om7j</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Help with booking an appointment please?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aqbbbttrrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1m3ogvv</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>First time EVER doing tortie design</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/reb94c0cqrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1m3obx8</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>I recently changed from square round to oval and I’m really happy with it</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u3ne3s3uordf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1m3nzx8</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Fake Toenail question</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3nzx8/fake_toenail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1m3nshx</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1iy4vz9jrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1m3n29f</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Western theme I did today 🌵🐮</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hemrnxhwbrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1m3mmkg</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>My second time getting nail art done. Full of stuff i like</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3mmkg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1m3lxnc</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Ceramic Fruits</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3lxnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1m3m41o</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Fingernail curves</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tax1uqn2rdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1m3m40a</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>In love with princess nails 🩵✨</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edscv93o2rdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1m3m1xt</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>first ever set of nails!</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s2umhx42rdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1m3lt02</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Sometimes You Just Need a Little Colour—Short Almond Nails 🌈💅</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3lt02</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1m3lprw</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>My new nails!!! I’m in love</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3lprw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1m3lluj</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Nail day new press ons</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3lluj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1m3ko91</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>someone please gaslight me into liking these</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ko91</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1m3kdsc</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Does this color look bad??</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3kdsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1m3k5u3</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>made some maggot nails :)</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqxtw6hqkqdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1m3k3z7</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>A glitter manicure for the sun to be even brighter</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yf9ur495kqdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1m3k05h</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Pastel marbling 🥰</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3k05h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1m3jyug</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Simple but they bring me so much joy 🥹</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3jyug</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1m3johy</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Monkeys!</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3johy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1m3j4cx</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My beach day nails. I’m so proud of it</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3j4cx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1m3itau</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>how to fix</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3itau</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1m3iyjg</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Advice for DIY press-ons?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3iyjg/advice_for_diy_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1m3is98</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>my fruit salad nails 🍇</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mztq7ehi8qdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1m3imm6</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Press on nails</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r1v90g337qdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1m3hil4</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Best LED/UV nail lamp..</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3hil4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1m3ht20</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Concert nails😍</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kcnpih470qdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1m3hr7x</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Update: at home, real nails, french manicure! (2nd time doing this)</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3hr7x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1m3hqo1</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3hqo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1m3h45x</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Love these 3d cherries!</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tesz26klupdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1m3gy8o</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Strawberry Nails🍓</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4d1fk49tpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1m3gy54</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Broken Nail :-( What would you do?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4hcrh48tpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1m3gwij</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Nail art troubles</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3gwij/nail_art_troubles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1m3gocv</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>What I got VS what I asked for! Summer nails 🌞 inspo from Pinterest</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3gocv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1m3gpob</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Medieval Nails</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jt3q2ledrpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1m3gbn4</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>I am working on teaching myself how to do my own nails at home. These are my natural nails, and for some reason I just don’t quite like this shape right now even though it’s normally a favorite of mine. Any suggestions on other shape options that I can change it to without losing much length?</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ukwzk9ncopdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1m3g6h8</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Last nail design for a while</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzh9sbr6npdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1m3fq3n</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>My first press-on set I made. (Inspired from a pic on Pinterest) Hoping they stay on for a while! Any glue recommendations?</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3fq3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1m3g470</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>long nail help</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3g470/long_nail_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1m3ecgc</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Why won't my nails stay on?</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3ecgc/why_wont_my_nails_stay_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1m3fohd</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>I handpainted shroomies!</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ww0ffkhajpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1m3f1u3</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Does contact dermatitis go away?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3f1u3/does_contact_dermatitis_go_away/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1m3fy1f</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Gel Press ons Set for my Bestie’s Bday🐚✨🌊</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3fy1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1m3fspu</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Just a flawless French 💅</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx2yfns6kpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1m3frr7</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Materials for start doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3frr7/materials_for_start_doing_my_own_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1m3fqwz</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Mint green 💚</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3fqwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1m3eysv</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>First time trying nail art- Jurassic Park 3 nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ym5z1eevdpdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1m3epq4</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>First “independent” attempt on Russian manicure.</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0hw9akuzbpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1m3e51a</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>My nail tech absolutely killed it with this set. I'm in love❤️</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3e51a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1m3e4i2</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Is there a way to make the free edge on the sides of my thumbs go away? Like how can the nail bed grow instead?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3e4i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1m3dxsp</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>I love nails , but taking them off is sooooo much work</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9tfuon96pdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1m3b6us</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Dog cracked side of my nail and I have no idea how to treat it</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3b6us/dog_cracked_side_of_my_nail_and_i_have_no_idea/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1m3d3lq</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Zoya - Thandie</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3d3lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1m3d2v7</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>🌺</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j4tja5o10pdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1m3cubf</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Fun pastel rainbow nails with frog</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0zsazbayodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1m3cjgl</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>First time getting neon nails</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qe7cw454wodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1m3chbb</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Latest set</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o6pkg2pvodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1m3cbnz</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Cheeky cheetah! 🐆</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6qzvzaluodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1m3c9z4</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Blooms 🌸</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k0vqms79uodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1m3c6n4</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>I really like my new set 🥰</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3c6n4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1m3c5wu</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Some Snoopy nails I’ve made</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3c5wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1m3bxnd</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Got my nails done. What do you think?</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyct9o5srodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1m3bg5m</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>love these nails so much🎀✨</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5j1s7k9oodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1m3bsvc</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Yall do we like the new set (it’s press ones btw)</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3powndxtqodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1m3bav5</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>My nail tech can do anything</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3bav5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1m3a79c</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Gel allergy, would just acrylic and OG nail polish work?</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3a79c/gel_allergy_would_just_acrylic_and_og_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1m3ax7u</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Is there a name for this type of design?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ax7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1m3airm</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Got my nails done for a Spiderman themed party</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x19y2utqhodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1m3ahp8</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Wanted something ✨sparkly✨</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2zu0ivzjhodf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1m3aci2</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Summer pink Pool vibes</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3aci2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1m3a6p4</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Vacation ready 🦋☀️🏖️</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ak2n7qrefodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1m39wnr</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>Some tamagotchi nostalgics in the room?</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m39wnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1m39sds</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Loveee my nail tech🫶🏽😭</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m39sds</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1m39ro7</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Do you like the mix of colors? Improvise</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ezv29p2kcodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1m39do5</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Glitter for cuticle oil?</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m39do5/glitter_for_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1m3932c</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Does anyone know how I can go about fixing this snagged nail?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u15o4o8v7odf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1m391vs</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Acrylic marker nails</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m391vs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1m38xoo</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>I just started doing my own nails</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m38xoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1m38o0k</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>What should I ask for in the salon?</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h5sgyggz4odf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1m38im0</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Why won't the salon give me pointed nails?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m38im0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1m38q7a</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>First couple gel x sets</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m38q7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1m38i5p</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>I got new nails yesterday! 💅🏼 do we like them?? Please be nice haha</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m38i5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1m384p3</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Starry Skies 😊</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dh9s038d1odf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1m382ku</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>I asked for Demon Slayer nails for my birthday</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnwuk3mz0odf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1m380jl</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>are they white or blue??</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m380jl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1m37mgk</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Natural Nail Growth ~6 weeks</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pgm9y31yndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1m37pyt</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>White felt so plain I added an accent nail</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pg16i0qoyndf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1m37nrh</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Rainbow tips</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m37nrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1m37hy0</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Struggling to get the perfect oval shape</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m37hy0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1m370zy</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Short natural nails in cool toned blue</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/karzgb9wtndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1m36s80</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Obsessed with this set</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m36s80</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1m36j5r</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Obsessed with this style for summer</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m36j5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1m3620x</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Lemon nails for Summer 🍋</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3620x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1m35yeo</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Wanted to show some strawberry nails I made.</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0couibfmndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1m3qvme</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Superman! 💙❤</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lc09v9n5hsdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1m3qu8k</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>My first nail art was inspired by my favourite cardi</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/am0fkqepgsdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1m3pp0g</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Toil and Trouble with mani mags</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3pp0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1m3pbhv</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Found a perfect polish + holo combo</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2do8qxsizrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1m3p0mf</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>How can I prevent these cuticles from growing back so fast?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydk583bvvrdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1m3ovkz</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>{PR} Kickin’ It With My Offs On (Exclusive – PBE 2025)</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ovkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1m3ogld</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Seeking flakie bombs!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3ogld/seeking_flakie_bombs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1m3oanu</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>What is this magicalness?!</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0gz04wigordf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1m3oa6a</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>{PR} Taylor Street – Sassy Sauce Polish (PBE Exclusive)</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3oa6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1m3ni7d</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Fall colors in summer</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ni7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1m3nael</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>{PR} Northerly Island Nights - Sassy Sauce - PBE</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3nael</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1m3n3ii</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Disappointed</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3n3ii</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1m3lshp</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>1st plain jelly, 1st Starrily</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3lshp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1m3lmbl</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>I have a lot of trouble getting nails to stay and glue on when I use a stand</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>/r/GelX_Nails/comments/1m3ljz7/i_have_a_lot_of_trouble_getting_nails_to_stay_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1m3lm38</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Any advice on how to achieve this</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejf3j4b0yqdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1m3lf5j</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Can you tell what it's supposed to be?</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0yigdun8wqdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1m3kvks</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>ILNP Mega(S) 💅 is holo perfection</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0af9u2x6rqdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1m3ko5p</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>First BKL order and it was love at first swatch</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ko5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1m3ko55</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>New to this hobby: Manis of the week</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ko55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1m3kb9r</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>HAUL! Long  time lurker👀finally convinced to check out the nail section at my  local Dollar Trees &amp; Dollar Generals</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3kb9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1m3jnbl</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Fancy Gloss colorful magnetic toppers</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3jnbl/fancy_gloss_colorful_magnetic_toppers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1m3jdun</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Barney Vibes</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s98w6hjtdqdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1m3jbr9</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Oooo I feel fancy ❤️</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1snlr8bdqdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1m3jbiu</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Does BKL ever restock sold out colors?</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3jbiu/does_bkl_ever_restock_sold_out_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1m3isf8</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>BR Little Prince vs BKL Feo, Fuerte y Formal</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3isf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1m3irvv</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>BR Little Prince vs BKL Feo, Fuerte y Formal</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3irvv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1m3im9d</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>Looking for suggestions</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz8888v27qdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1m3howh</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Met a lacquerista in the wild and she wasn’t excited :’(</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3howh/met_a_lacquerista_in_the_wild_and_she_wasnt/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1m3hlh5</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Please help me find a polish like the iridescent pink/purple/blue above the birb's wing (thank you)</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyqw244tyfdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1m3h8qz</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Summer is for violently neon shorties 💚</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3h8qz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1m3h5uk</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Sometimes you just gotta embrace the inner witch 🦇🖤</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3h5uk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1m3gyd5</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>I was trying to go for the colors of sunset</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tmv85ax9tpdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1m3grpm</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Mermaid nails 🩵💚💜🩷</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3grpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1m3gpot</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Can you please help me pick a nude-tral? Please?</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3gpot</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1m3g5oq</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>ABC of polish- Y</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9v36cj0npdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1m3fkjk</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>chaos skittle 🌌🌳🌈🍓✨</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3fkjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1m3f9xc</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Bees Knees - Curious about today's drop (first time buyer)</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3f9xc/bees_knees_curious_about_todays_drop_first_time/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1m3f8o3</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Shipping to Europe</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>/r/CirqueColors/comments/1m3f65s/shipping_to_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1m3e6de</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>I'm in love! 💖</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3e6de</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1m3e2sq</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Still have to learn how to take pictures of my nails 💖 (ft. blurry background kitty!)</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyzymxy97pdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1m3dxs0</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>A glossy surprise</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g0r5vie96pdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1m3ddnm</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>ISO Black Green</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3ddnm/iso_black_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1m3crc7</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>8 months' progress!</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3crc7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1m3cj5a</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Someone on r/NailArt told me I should post here my new nails!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q5mkq432wodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1m3cfjo</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>The first two polish colors in this video</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3cfjo/the_first_two_polish_colors_in_this_video/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1m3by22</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Mooncat’s Fields of Lavender</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u3veo5purodf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1m3bq9v</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Sharpened my claws</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/95id9azaqodf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1m3bdqo</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Just have to show off Seawinkle before I take it off ♡</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3bdqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1m3bc5t</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>Anyone know if Ethereal Lawyers Howls Moving Castle collection ever coming back?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3bc5t/anyone_know_if_ethereal_lawyers_howls_moving/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1m3an8v</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>my HHC came in</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sjy2fv6kiodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1m3adrs</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>An oldie but a goodie: Butter London Victoriana</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3adrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1m3a9ge</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>How do I stop deep sidewall tears on my thumbs? (Typing-related?)</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3a9ge/how_do_i_stop_deep_sidewall_tears_on_my_thumbs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1m3a6xe</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>To nip or not to nip?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3a6xe/to_nip_or_not_to_nip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1m3a28m</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Trying to dupe Mooncat Forces of Evil with things that aren’t limited edition or discontinued yet</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b20uhc8leodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1m39uwg</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Nebula</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xufisq06dodf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1m39mu7</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Non-gel nail tip alternatives for using as press-ons with acrylic nail polish?</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m39mu7/nongel_nail_tip_alternatives_for_using_as/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1m39hu0</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>2022 &gt; 2024 &gt; Now</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m39hu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1m3930e</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Shimmering in sunlight &amp; shadows ✨☀️🌒</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rtyhhtmu7odf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1m38t7s</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Not usually an orange gal but this one is surprisingly fun</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flinrw7z5odf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1m36qp9</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Birthday + Pride in July 🌈</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m36qp9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1m365mu</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>i'm new here, any tips?</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m365mu/im_new_here_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1m363ej</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>the fomo got me…</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dglkhrbfnndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1m35uc0</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>🩵💜Vibrant Stripes🧡💛</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m35uc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1m352lu</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>ILNP summer gradient</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m352lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1m33t4u</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Nicole Miller minis?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m33t4u/nicole_miller_minis/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1m33dul</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Cirque Colors Birthday Sale Haul</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m33dul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1m32p1p</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>First time doing my nails 🐣</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m32p1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1m32e1z</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>(Un)Guilty Pleasures + Gilded Galaxy Essie combo</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtnvkg6dxmdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1m327sw</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Primary colors + a lil’ gem</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m327sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1m31kvy</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>My first attempt at nail art</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/03j1x1q2rmdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1m312md</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Assymetric mani with waves and koi</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m312md</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1m311qj</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Has anyone tried these Kiko nail polishes? the colors look nice</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ybkverjmmmdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1m30t7e</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m30t7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1m2z2ii</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>☕️🐻🍫</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fad0n6ce4mdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1m2ylvx</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Follow-up on Essence Glossy Jelly</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2ylvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1m2y5db</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Better quality dupe for Sally Hansen - Bamboost? (UK)</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8sl50tr7uldf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1m2xl3o</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Told my sweet boyfriend I was going to finally buy a horseshoe magnet for nail polish. He said "I got you, babe". I received this in the mail today 😆❤️</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m2xl3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1m2wzf3</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>What exactly is Unicorn Pee</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2wzf3/what_exactly_is_unicorn_pee/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1m2wp4t</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Is it possible to be allergic to HEMA free polish?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m2wp4t/is_it_possible_to_be_allergic_to_hema_free_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1m3q3q2</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>French Gel Polish</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw1fkmse8sdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1m3n3na</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Western theme I did today 🌵🐮</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vx2vkrfacrdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1m3aczr</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Made press ons for the first time for my friend for vacation !!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zty2otwngodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1m3m3st</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Tropical vibe 🌴🍹</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4vm182m2rdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1m3ltq8</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Life’s Better with Colour! Here’s a Fun Short Almond Set</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ltq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1m3ksfp</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Neon laserbeams</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ksfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1m3j3nw</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>She wanted edgy nails…</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3j3nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1m3ihtd</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>These nails took me 12 hours ngl 🌸</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c61rjd7r5qdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1m3cytf</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>My Nails atm :)</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3cytf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1m3csuj</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Nails I made for MN ritual 8/2 :D</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6xtbd4txodf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1m3c4ax</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Small business nail charms</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m3c4ax/small_business_nail_charms/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1m3ay1r</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>show me what you got 👁️👄👁️ … i have a plumbus</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3ay1r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1m39z30</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Any tamagotchi nostalgics in the room</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m39z30</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1m3849c</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Crystal Galaxy Vibes</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qlpxf6fa1odf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1m37hwf</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gzrmc786xndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1m35zov</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Made some strawberry nails</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xfnflyomndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1m35nce</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Summer ice nails - I absolutely love them!</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m35nce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1m339kq</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>show me your current practice nails ! :) here's mine, trying to get good at 3d flowers and cursive.</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m339kq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1m33015</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>be honest does this look okay</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6sjodyx1ndf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1m32gqs</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Shipwreck nails</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m32gqs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1m31j2z</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Cute little fish for summer 🐟</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m31j2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1m30vze</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>The before and after I’m more than proud of</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m30vze</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jul 20 08:11:59 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_07_20.xlsx
+++ b/data/collected_data/2025_07_20.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1320"/>
+  <dimension ref="A1:C1532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22873,6 +22873,3610 @@
         </is>
       </c>
     </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1m4j2to</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Nail shape advice needed!</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e40d551jgzdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1m4itmj</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Do you believe in Aliens? 👽😜</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3rbuihlhdzdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1m4hv3u</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>First time cat-eye</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/reh5a4bq2zdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1m4husu</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Rate</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rvjozr3l2zdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1m4gxej</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>I love y'all!</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4gxej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1m4hdm8</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Fresh new set</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f0dzyjwfxydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1m4h9c4</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Best press on nail brand for wide fingernails???</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m4h9c4/best_press_on_nail_brand_for_wide_fingernails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1m4h11u</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Why is there blue on my nails all of a sudden?!</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyzj8vvmtydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1m4gdx2</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>My last job of the day</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzfvajismydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1m4gbo2</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>I feel like I finally found the perfect beige/pink 😍</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ld8776k4mydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1m4g3ye</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Trialing birthday nails. Swipe to see color change + glow in the dark! 🌟</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4g3ye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1m4g682</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>New Cinnamoroll nails 🩵</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4g682</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1m4afkq</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Alternative to gel bc of allergy</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m4afkq/alternative_to_gel_bc_of_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1m4fqkc</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>yay or nay?</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6sn9382gydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1m4fp7n</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>love my new nails first time trying some red!</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kwhe95mofydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1m4fioj</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>What shape do I have?</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pu5i0keudydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1m4faco</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Malepolish</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4wdee94jbydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1m4f02l</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Nails for my cousin's wedding</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4f02l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1m4etod</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Fetus Nail</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4etod</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1m4emzr</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>New to Press Ons - what are my next steps? did I wreck my nails?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxfzs5965ydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1m4e1zh</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Can you get dip or acrylic if you react negatively to gel polish?</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m4e1zh/can_you_get_dip_or_acrylic_if_you_react/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1m4e1w8</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>OPI gel peels every time I get it</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kprqvdmlzxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1m4dhsh</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>First time doing press ons</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x63gdxgduxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1m4ddj0</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>In love with my new set!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ednf1gbatxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1m4d5u1</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>What long-lasting regular nail polish do you recommend?</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sr5encrcrxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1m4d4tg</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Strawberry naillss</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9miebo13rxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1m4d3la</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Watermelon swirl</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6gjlw7orqxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1m4czdj</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>fresh manicure and ready to conquer the world</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/asw7nhjkpxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1m4cj7v</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Today's work</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ayb190mlxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1m4bj6s</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>obsessed is an understatement</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/a58qga0hcxdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1m4bggi</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Looking for a specific color!!</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4bggi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1m4az3t</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>Press ons I made</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etw07jyj7xdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1m4aykm</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>I'm a beginner, I practice on myself</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3imspk1f7xdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1m4ax8f</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Twinkle twinkle little star</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7bboxzh37xdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1m49zdr</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Aspiring nail tech first practice set</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbunm6n7zwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1m49yxx</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Stained Glass Bachlorette Nails</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m49yxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1m49voe</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>First time making press on nails!</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m49voe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1m49ts5</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Encanto theme for a baby shower 🌺</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m49ts5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1m49i7f</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Board Game Nails</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/siuxs7vavwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1m48zji</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Nail lamp opinions, which ones do you prefer?l</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m48zji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1m48ggk</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Wish the foil was more vibrant but love this look!</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1pwnun8lmwdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1m48xxp</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>All the little bugs!</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m48xxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1m48x7u</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Total Beginner - what nail shape would look good with my natural nails, and other advice?</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m48x7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1m48l2d</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Thoughts on Essie Stay Longer Top Coat</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13lmms3onwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1m480mh</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>what i got vs what i asked for</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m480mh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1m47y3r</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Wanted cats eye, feel like I got "sparkly blue" am I wrong?</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ms9x2f0niwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1m47ufb</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>My vacation nails</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4yuwfx4thwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1m480i9</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Trying to figure out if nail shape supposed to match your finger type. Any suggestions?</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zeifnak5jwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1m47sch</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>has anyone connected two nails with a chain? two days in and it’s a lot more practical than i expected so i’m curious why i never see them</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rsduwbchwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1m45tuj</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Cracked vertically - what to do?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gnyy4uq22wdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1m44x58</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>do they look like they're.. idk inflamed?</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m44x58</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1m4604a</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>I think I did great with the mother of pearl inspired mani (Ignore the cuticles)</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4604a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1m467tr</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>New to gel and clumsy with regular, how do I keep excess polish off my skin?</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m467tr/new_to_gel_and_clumsy_with_regular_how_do_i_keep/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1m47ee9</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>Whats the knife included on some nailcutters for?</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m47ee9/whats_the_knife_included_on_some_nailcutters_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1m47gni</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>Sephora by OPI - metro chic</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m47gni</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1m4740e</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t>I️ Love Nail Polish!</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4740e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1m474az</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t>Padme nails round 2</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m474az</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1m475m1</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>weekend set 💎</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/81wi2ntdcwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1m46vcc</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>do you consider my nails to be long or short?</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tgiswn6awdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1m46smy</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Whats your favorite base color</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5kikjgg9wdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1m466ex</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>My nails two weeks ago</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k8yxga9q4wdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1m45ygz</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time in like 8 years and I can’t believe I went this long without such a treat! I got a pedi too and omg!</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m45ygz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1m45qus</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>“You Had Me At Confetti” by OPI has had me in a chokehold all summer long</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m45qus</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1m45iqn</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Gel X done by me</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m45iqn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1m45583</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>First Time Doing Designs on Nails</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66vgaktywvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1m43p0a</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>Casino Nails - what do you think?</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://youtube.com/shorts/5Lsek6nVdw4?si=mLX36Xvf1NTjaRJF</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1m44yc2</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Fruit &amp; Flowers: the perfect summer combo</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k30zsq5jvvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1m44vt0</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>First time getting gel x nails</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l2nw810vvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1m44d0g</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Bad habits from my parents</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m44d0g/bad_habits_from_my_parents/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1m44apz</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>I normally do long nails but I wanted some shorties this time for comfortability</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/889tsiknqvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1m449z6</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t>My nail lady blows it out of the park again. I'm in love with this set!</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ltyuzwhqvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1m446r2</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>A moment of appreciation for my slightly-stained moisturized nails</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kmkgn1ppvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1m44453</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>My new nail tech/artist succeeds again</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m44453</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1m43vgw</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Fish nails</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3pre27jnvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1m43nih</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>A rainy afternoon with not much to do…</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vxroc4zulvdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1m43ml0</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Wearing the cosmos on my nails ⭐️ 💜</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m43ml0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1m43bqk</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>Wasn’t sure how I felt about these, but they’re growing on me!! 🍋</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko7ngo2ijvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1m434xt</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Yay or Nay?</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xlf0lsd1ivdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1m433e0</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Work at home</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9o2lbddqhvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1m42bbc</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>Veggie Nail Art</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m42bbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1m41j5h</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Topcoat changing color of nails, help!</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfd9z5t56vdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1m3z147</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>My take on the butter nail trend</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3z147</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1m3yevk</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Nail health/ chemo</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3yevk/nail_health_chemo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1m41u46</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>DND Ferrari red vs opi big apple red?</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m41u46/dnd_ferrari_red_vs_opi_big_apple_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1m41nqk</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>new nails, shorter and less sharp cause i keep stabbing my own eyes while i sleep</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ftru4o37vdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1m41lxp</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Beach nails from a new to me independent tech!</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m41lxp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1m419zq</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Nails aren’t giving</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m419zq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1m40x19</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Summer Blues 🩵</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m40x19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1m40vwy</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Can acrylic fix a broken nail?</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m40vwy/can_acrylic_fix_a_broken_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1m40vbz</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Acrylics pop off after 2 weeks</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m40vbz/acrylics_pop_off_after_2_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1m40pj7</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>First time: 1. Working with polygel 2. Doing the Lazy Girl Method 3. Doing chrome (kindly ignore the chrome cuticles)</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0yyu1a30vdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1m3zu84</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Nails growing from sides</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edmlv9umtudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1m3zo50</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>Leftover residue and chipping on nails</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3zo50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1m3z9og</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>I’ve been experimenting making marble nails</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3z9og</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1m3z2zo</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjglh2t1oudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1m3yzmf</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Can never go wrong with a classic red ♥️</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9h58ywcnudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1m3xhsu</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>what shape are the nails that I got?</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3xhsu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1m3wpsn</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>These are from some months ago. What do we think??? Please be nice!! &lt;3 I loved them but then I got bored haha (inspo at the end)</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3wpsn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1m3wcgg</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>OPI GELement Starter Kit Best?</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb4b1ibs1udf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1m3wan7</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>How do i take off gel polish??</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1m3wan7/how_do_i_take_off_gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1m4ipyq</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>European non-drugstore polish hunting</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m4ipyq/european_nondrugstore_polish_hunting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1m4iiij</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>I felt inspired by garden and the critters I keep finding in it</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/maycv2j1azdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1m4i6do</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>Made my first ever set of press ons. Did I do okay?</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4i6do</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1m4hovn</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Caviar nails</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ql859180zdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1m4h6ut</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>I wanted to share my nail polish set up and collection!</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4h6ut</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1m4gk7c</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>Moth and Moon Soul</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/87cy78gloydf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1m4ft43</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Dry time between coats?</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4ft43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1m4fk1k</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>My Cirque Colors birthday gift to myself</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jikamu58eydf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1m4f6vp</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>I combined all my oranges and yellows onto one swatch ring, and my collection still looks like this 💀😆 Anyone else have a color family you just don't buy?</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18me60it8ydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1m4e2a5</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>How to get nails like these without gel</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4e2a5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1m4cndt</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Top coats for glow in the dark/UV polishes?</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m4cndt/top_coats_for_glow_in_the_darkuv_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1m4cnqp</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>help finding color dupe!</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4cnqp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1m4cb12</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>Thermal help</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m4cb12/thermal_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1m4c1y2</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>Can everyone see my screen</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4c1y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1m4bol4</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Amazing purple 💜👾</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3t3b5imvdxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1m4bmzh</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Flakie + Jelly = 💜</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tn4phdlgdxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1m4bej3</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Bon Voyage!</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5mrho7cbxdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1m4b1qm</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>When life throws dumpster fires at you, sharpen your claws, paint ‘em black, &amp; make ‘em matte 🖤</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4b1qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1m4aus8</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>The reflects make my brain feel funny</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n5gztvfj6xdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1m4aucd</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t>Vortex Mixer Recs</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m4aucd/vortex_mixer_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>1m4at0p</t>
+        </is>
+      </c>
+      <c r="B1441" t="inlineStr">
+        <is>
+          <t>The Living Usually Won't See the Dead</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4at0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>1m49r03</t>
+        </is>
+      </c>
+      <c r="B1442" t="inlineStr">
+        <is>
+          <t>It’s so shimmery!!</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m9rsblgaxwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>1m49p10</t>
+        </is>
+      </c>
+      <c r="B1443" t="inlineStr">
+        <is>
+          <t>Casualty of Poor Packaging</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2c4xwwrvwdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>1m49ncb</t>
+        </is>
+      </c>
+      <c r="B1444" t="inlineStr">
+        <is>
+          <t>Wearing the cosmos on my nails ⭐️ 💜</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m43ml0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>1m49ho9</t>
+        </is>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Potion Polish is having a sale this weekend.</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m49ho9/potion_polish_is_having_a_sale_this_weekend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>1m4989y</t>
+        </is>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Glitter french tips</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4989y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>1m496hp</t>
+        </is>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>all I can say is wow</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02px8w2mswdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>1m494n5</t>
+        </is>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>You Had Me at Aloha</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m494n5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>1m48cje</t>
+        </is>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Oooooo Shiny</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m48cje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>1m4702a</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>I️ Love Nail Polish!</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4702a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>1m46fvt</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Fancy✨🪄🧚🏻</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m46fvt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>1m46e0c</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Lacquer on toe skin vs on finger skin</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m46e0c/lacquer_on_toe_skin_vs_on_finger_skin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>1m45m7q</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Dragon Fly 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iecry5ei0wdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>1m4588w</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>gray tabby love 🐱</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4588w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>1m44tel</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>ILNP Rosewood vs Essie Never Basic - any examples?</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m44tel/ilnp_rosewood_vs_essie_never_basic_any_examples/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>1m44bdn</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>30 lb Magnet vs 20 lb Magnet</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7vxuy6fsqvdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>1m44513</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>OBSESSED with My Bugs! My Bugs! and how bright my nails glow</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m44513</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>1m442gq</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Showoff</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m442gq/showoff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>1m4413g</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Baronial Nail Art</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4413g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>1m43k5y</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>[Sassy Sauce Polish – Yayyy You’re Here 2025 | PBE Exclusive]</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m43k5y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>1m43gnr</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>What is your favorite tab opener?</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m43gnr/what_is_your_favorite_tab_opener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>1m42lay</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Cherry Checkerboard Nails 🍒</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yi98nuy5avdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>1m42j47</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Tips and tricks for water marbling?</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m42j47</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>1m41uc0</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Goddess of Rays</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m41uc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>1m413gr</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Baby boomer style nails but make it magnetic</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xfiwowqy2vdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>1m412et</t>
+        </is>
+      </c>
+      <c r="B1466" t="inlineStr">
+        <is>
+          <t>Monarch Lacquer FTW</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ngswdn2r2vdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>1m40pol</t>
+        </is>
+      </c>
+      <c r="B1467" t="inlineStr">
+        <is>
+          <t>Diffused glass beads!</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bxyzq5t30vdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>1m38amk</t>
+        </is>
+      </c>
+      <c r="B1468" t="inlineStr">
+        <is>
+          <t>I Invoke Thee, Bee's Knees 🔮</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p65n1bs62odf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>1m3f3ev</t>
+        </is>
+      </c>
+      <c r="B1469" t="inlineStr">
+        <is>
+          <t>Nail art fail</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3f3ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>1m3hz72</t>
+        </is>
+      </c>
+      <c r="B1470" t="inlineStr">
+        <is>
+          <t>Vintage sinful and California colors</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1jyr2s2n1qdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>1m3y29u</t>
+        </is>
+      </c>
+      <c r="B1471" t="inlineStr">
+        <is>
+          <t>Baja be thy blast 🙏</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3y29u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>1m40g0b</t>
+        </is>
+      </c>
+      <c r="B1472" t="inlineStr">
+        <is>
+          <t>0 days without incident 😭</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tktxzh64yudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>1m402om</t>
+        </is>
+      </c>
+      <c r="B1473" t="inlineStr">
+        <is>
+          <t>I have very stained nails because of a red polish (I used the base), but I would like to use a sheer polish, how can I do it without the color of my nails affecting the color of the nail polish??</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m402om/i_have_very_stained_nails_because_of_a_red_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>1m4028r</t>
+        </is>
+      </c>
+      <c r="B1474" t="inlineStr">
+        <is>
+          <t>What is too warm for polish storage?</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m4028r/what_is_too_warm_for_polish_storage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>1m3zwwo</t>
+        </is>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Brown magnetic over red turned into a beautiful copper 🤎</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3zwwo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>1m3zsuq</t>
+        </is>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Olive Ave Polish sale</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aulwmd3dtudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>1m3zot9</t>
+        </is>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>[PBE 2025 Exclusive] What the Helley by Sassy Sauce 💗🖤</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3zot9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>1m3znu2</t>
+        </is>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>This just might be my favorite 1-coat crème blue 💙</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3znu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>1m3zk2m</t>
+        </is>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>I love toppers so much.</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3zk2m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>1m3zd0j</t>
+        </is>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Has anybody used a peely base coat for pedicures?  I like my toes to match my nails but I hate doing pedicures! Wondering how long it would last in summer wearing only sandals.</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3zd0j/has_anybody_used_a_peely_base_coat_for_pedicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>1m3z9fw</t>
+        </is>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>My Ugliest Manicure Yet!</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/19pjysdepudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>1m3z2ni</t>
+        </is>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Nail growth tips?</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jtm977znudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>1m3yna2</t>
+        </is>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Bees Knees Lacquer Arcana</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kh98r4vnkudf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>1m3y5f6</t>
+        </is>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Pls help with glass bead</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/olr5qj4nfudf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>1m3y43o</t>
+        </is>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>my answer to my long hot dog nails, I give you short hamburgers</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh5ard4rgudf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>1m3y06u</t>
+        </is>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Sparkles are my fave 💜</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3y06u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>1m3vwoi</t>
+        </is>
+      </c>
+      <c r="B1487" t="inlineStr">
+        <is>
+          <t>Some Bird and Botanical Nails</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3vwoi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>1m3vlrn</t>
+        </is>
+      </c>
+      <c r="B1488" t="inlineStr">
+        <is>
+          <t>What can I do about the pain?</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3vlrn/what_can_i_do_about_the_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>1m3vkhi</t>
+        </is>
+      </c>
+      <c r="B1489" t="inlineStr">
+        <is>
+          <t>🍋🩷Neon Pink Lemonade🩷🍋</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3vkhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>1m3upfx</t>
+        </is>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Do you know a green polish in any of these green shades?</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kj0rl82otdf1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>1m3tebm</t>
+        </is>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Essie - Bikini So Teeny (UK edition)</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3tebm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>1m3tbwe</t>
+        </is>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>What would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3tbwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>1m3t4zq</t>
+        </is>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Too much thinner and how long to wait to evaporate?</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1m3t4zq/too_much_thinner_and_how_long_to_wait_to_evaporate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>1m3sx6z</t>
+        </is>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>I went on vacation and came back with these.</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yp6k3p2k5tdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>1m3spcj</t>
+        </is>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Clipoers/Nippers</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/momewgwy2tdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>1m3scvm</t>
+        </is>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>In a pink kinda mood 🩷</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3scvm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>1m3r39k</t>
+        </is>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>Kryptonite 💚💚 (plus glow in the dark)</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3r39k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>1m4izf6</t>
+        </is>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Beach vacation nailart</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjlt9soefzdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>1m4is9o</t>
+        </is>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Do you believe in aliens? 👽😜</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7ziku1b1dzdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>1m44bji</t>
+        </is>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Boyfriend nails as amateur artist</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m44bji</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>1m4h6fy</t>
+        </is>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Miffy!</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/207ay02avydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>1m4geki</t>
+        </is>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>My last job of the day</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rvxu2gzmydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>1m4gay2</t>
+        </is>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>Working on some Naruto nails — would love your feedback!</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4gay2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>1m4fzha</t>
+        </is>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>One of my favorite sets 🌊☀️</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcmsmjqmiydf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>1m4e1gu</t>
+        </is>
+      </c>
+      <c r="B1505" t="inlineStr">
+        <is>
+          <t>7 months of no biting and I found a new hobby out of it (progress)</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4e1gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>1m4ci9g</t>
+        </is>
+      </c>
+      <c r="B1506" t="inlineStr">
+        <is>
+          <t>Today's work</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkto0atclxdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>1m4b8eq</t>
+        </is>
+      </c>
+      <c r="B1507" t="inlineStr">
+        <is>
+          <t>Fairy Garden Inspired 🧚‍♀️</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4b8eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>1m4b73s</t>
+        </is>
+      </c>
+      <c r="B1508" t="inlineStr">
+        <is>
+          <t>Shrimps is bugs</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6op0rwdi9xdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>1m4aeno</t>
+        </is>
+      </c>
+      <c r="B1509" t="inlineStr">
+        <is>
+          <t>Update for the Glitter Gladiators! What do ya think? Did we do the right thing? Too much? Or not enough?</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m4aeno</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>1m46eg3</t>
+        </is>
+      </c>
+      <c r="B1510" t="inlineStr">
+        <is>
+          <t>Megz inspired set</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m46eg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>1m457lv</t>
+        </is>
+      </c>
+      <c r="B1511" t="inlineStr">
+        <is>
+          <t>Bach trip diy</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m457lv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>1m44r1b</t>
+        </is>
+      </c>
+      <c r="B1512" t="inlineStr">
+        <is>
+          <t>First time designs</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qfws2sv0uvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>1m44paj</t>
+        </is>
+      </c>
+      <c r="B1513" t="inlineStr">
+        <is>
+          <t>Zelletten Fussel nach Cleaner</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1m44paj/zelletten_fussel_nach_cleaner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>1m44ocd</t>
+        </is>
+      </c>
+      <c r="B1514" t="inlineStr">
+        <is>
+          <t>Liner brush improvement</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m44ocd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>1m447hs</t>
+        </is>
+      </c>
+      <c r="B1515" t="inlineStr">
+        <is>
+          <t>Do you normally plan your design or just start and see where you end up?</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q91jwimxpvdf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>1m447il</t>
+        </is>
+      </c>
+      <c r="B1516" t="inlineStr">
+        <is>
+          <t>Just wanted to show off my work, any critique is welcome</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qnzul5dzpvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>1m444ak</t>
+        </is>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>Under the sea…</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m444ak</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>1m43t0h</t>
+        </is>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>A quick set for the weekend</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0tpegiwmvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>1m434kp</t>
+        </is>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>New client</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qegx917zhvdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>1m42cvn</t>
+        </is>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Veggie Nail Art</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m42cvn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>1m425go</t>
+        </is>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Press on</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m425go</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>1m3qnz7</t>
+        </is>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>Look at the nails I made</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdahrwpresdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>1m3zg9c</t>
+        </is>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>My try with marble nails</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3zg9c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>1m3yn2g</t>
+        </is>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Gingham nails!</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3yn2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>1m3y8i7</t>
+        </is>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Cosmic Botanica</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/02z3smuohudf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>1m3y55d</t>
+        </is>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>I’m a chrome addict!!!!</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cx9gvu5ygudf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>1m3xp8l</t>
+        </is>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>First time ever doing nail art... kinda looks like shit but i feel sexy and gothic lol (included my inspo at the end)</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3xp8l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>1m3xmms</t>
+        </is>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>Doodle nails ✍️</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3xmms</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>1m3xc4l</t>
+        </is>
+      </c>
+      <c r="B1529" t="inlineStr">
+        <is>
+          <t>One Piece</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3xc4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>1m3te55</t>
+        </is>
+      </c>
+      <c r="B1530" t="inlineStr">
+        <is>
+          <t>First time attempting nail art (please read text for context)</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3te55</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>1m3t97z</t>
+        </is>
+      </c>
+      <c r="B1531" t="inlineStr">
+        <is>
+          <t>Still learning to work with gel polish</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1m3t97z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>1m3scle</t>
+        </is>
+      </c>
+      <c r="B1532" t="inlineStr">
+        <is>
+          <t>DIY gel nail art</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k80zdjhvysdf1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>